<commit_message>
Changed all Flags to Integers
</commit_message>
<xml_diff>
--- a/Database Data.xlsx
+++ b/Database Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylwa\source\repos\CIS424_wi21_Med_Cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D95290D-48E5-48B6-96DD-DA993E4FF3AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F316DE15-4202-419D-9870-04FFAF317DB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="718">
   <si>
     <t>User_ID</t>
   </si>
@@ -2556,8 +2556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2604,7 +2604,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
-      <c r="I1" s="4"/>
+      <c r="I1" s="11"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -2670,6 +2670,9 @@
       <c r="H2" t="s">
         <v>7</v>
       </c>
+      <c r="I2" t="s">
+        <v>574</v>
+      </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -2729,10 +2732,13 @@
       <c r="F3" t="s">
         <v>194</v>
       </c>
-      <c r="G3" t="b">
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" t="b">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>0</v>
       </c>
       <c r="K3" s="5"/>
@@ -2795,11 +2801,14 @@
       <c r="F4" t="s">
         <v>669</v>
       </c>
-      <c r="G4" t="b">
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" t="b">
+      <c r="H4">
         <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="6"/>
@@ -2861,10 +2870,13 @@
       <c r="F5" t="s">
         <v>670</v>
       </c>
-      <c r="G5" t="b">
+      <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" t="b">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>0</v>
       </c>
       <c r="K5" s="5"/>
@@ -2927,10 +2939,13 @@
       <c r="F6" t="s">
         <v>671</v>
       </c>
-      <c r="G6" t="b">
+      <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" t="b">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>0</v>
       </c>
       <c r="K6" s="5"/>
@@ -2993,10 +3008,13 @@
       <c r="F7" t="s">
         <v>672</v>
       </c>
-      <c r="G7" t="b">
+      <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" t="b">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>0</v>
       </c>
       <c r="K7" s="5"/>
@@ -3059,11 +3077,14 @@
       <c r="F8" t="s">
         <v>673</v>
       </c>
-      <c r="G8" t="b">
+      <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" t="b">
+      <c r="H8">
         <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="6"/>
@@ -3125,10 +3146,13 @@
       <c r="F9" t="s">
         <v>674</v>
       </c>
-      <c r="G9" t="b">
+      <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" t="b">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>0</v>
       </c>
       <c r="K9" s="5"/>
@@ -3191,10 +3215,13 @@
       <c r="F10" t="s">
         <v>675</v>
       </c>
-      <c r="G10" t="b">
+      <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10" t="b">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>0</v>
       </c>
       <c r="K10" s="5"/>
@@ -3257,10 +3284,13 @@
       <c r="F11" t="s">
         <v>676</v>
       </c>
-      <c r="G11" t="b">
+      <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11" t="b">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <v>0</v>
       </c>
       <c r="K11" s="5"/>
@@ -3323,10 +3353,13 @@
       <c r="F12" t="s">
         <v>677</v>
       </c>
-      <c r="G12" t="b">
+      <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12" t="b">
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
         <v>0</v>
       </c>
       <c r="K12" s="5"/>
@@ -3389,10 +3422,13 @@
       <c r="F13" t="s">
         <v>678</v>
       </c>
-      <c r="G13" t="b">
+      <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" t="b">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
         <v>0</v>
       </c>
       <c r="K13" s="5"/>
@@ -3455,11 +3491,14 @@
       <c r="F14" t="s">
         <v>679</v>
       </c>
-      <c r="G14" t="b">
+      <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14" t="b">
+      <c r="H14">
         <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="6"/>
@@ -3521,10 +3560,13 @@
       <c r="F15" t="s">
         <v>680</v>
       </c>
-      <c r="G15" t="b">
+      <c r="G15">
         <v>0</v>
       </c>
-      <c r="H15" t="b">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
         <v>0</v>
       </c>
       <c r="K15" s="5"/>
@@ -3587,11 +3629,14 @@
       <c r="F16" t="s">
         <v>681</v>
       </c>
-      <c r="G16" t="b">
+      <c r="G16">
         <v>1</v>
       </c>
-      <c r="H16" t="b">
+      <c r="H16">
         <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
@@ -3653,10 +3698,13 @@
       <c r="F17" t="s">
         <v>682</v>
       </c>
-      <c r="G17" t="b">
+      <c r="G17">
         <v>1</v>
       </c>
-      <c r="H17" t="b">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
         <v>0</v>
       </c>
       <c r="K17" s="5"/>
@@ -3719,10 +3767,13 @@
       <c r="F18" t="s">
         <v>683</v>
       </c>
-      <c r="G18" t="b">
+      <c r="G18">
         <v>1</v>
       </c>
-      <c r="H18" t="b">
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
         <v>0</v>
       </c>
       <c r="K18" s="5"/>
@@ -3785,10 +3836,13 @@
       <c r="F19" t="s">
         <v>684</v>
       </c>
-      <c r="G19" t="b">
+      <c r="G19">
         <v>1</v>
       </c>
-      <c r="H19" t="b">
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
         <v>0</v>
       </c>
       <c r="K19" s="5"/>
@@ -3851,10 +3905,13 @@
       <c r="F20" t="s">
         <v>685</v>
       </c>
-      <c r="G20" t="b">
+      <c r="G20">
         <v>0</v>
       </c>
-      <c r="H20" t="b">
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
         <v>0</v>
       </c>
       <c r="K20" s="5"/>
@@ -3917,10 +3974,13 @@
       <c r="F21" t="s">
         <v>686</v>
       </c>
-      <c r="G21" t="b">
+      <c r="G21">
         <v>0</v>
       </c>
-      <c r="H21" t="b">
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
         <v>0</v>
       </c>
       <c r="K21" s="5"/>
@@ -3983,10 +4043,13 @@
       <c r="F22" t="s">
         <v>687</v>
       </c>
-      <c r="G22" t="b">
+      <c r="G22">
         <v>0</v>
       </c>
-      <c r="H22" t="b">
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
         <v>0</v>
       </c>
       <c r="K22" s="5"/>
@@ -4049,11 +4112,14 @@
       <c r="F23" t="s">
         <v>688</v>
       </c>
-      <c r="G23" t="b">
+      <c r="G23">
         <v>0</v>
       </c>
-      <c r="H23" t="b">
+      <c r="H23">
         <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="6"/>
@@ -4115,11 +4181,14 @@
       <c r="F24" t="s">
         <v>689</v>
       </c>
-      <c r="G24" t="b">
+      <c r="G24">
         <v>0</v>
       </c>
-      <c r="H24" t="b">
+      <c r="H24">
         <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="6"/>
@@ -4181,11 +4250,14 @@
       <c r="F25" t="s">
         <v>690</v>
       </c>
-      <c r="G25" t="b">
+      <c r="G25">
         <v>0</v>
       </c>
-      <c r="H25" t="b">
+      <c r="H25">
         <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="6"/>
@@ -4247,11 +4319,14 @@
       <c r="F26" t="s">
         <v>691</v>
       </c>
-      <c r="G26" t="b">
+      <c r="G26">
         <v>0</v>
       </c>
-      <c r="H26" t="b">
+      <c r="H26">
         <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="6"/>
@@ -4313,11 +4388,14 @@
       <c r="F27" t="s">
         <v>692</v>
       </c>
-      <c r="G27" t="b">
+      <c r="G27">
         <v>0</v>
       </c>
-      <c r="H27" t="b">
+      <c r="H27">
         <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="6"/>
@@ -4379,10 +4457,13 @@
       <c r="F28" t="s">
         <v>693</v>
       </c>
-      <c r="G28" t="b">
+      <c r="G28">
         <v>0</v>
       </c>
-      <c r="H28" t="b">
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
         <v>0</v>
       </c>
       <c r="K28" s="5"/>
@@ -4445,10 +4526,13 @@
       <c r="F29" t="s">
         <v>694</v>
       </c>
-      <c r="G29" t="b">
+      <c r="G29">
         <v>1</v>
       </c>
-      <c r="H29" t="b">
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
         <v>0</v>
       </c>
       <c r="K29" s="5"/>
@@ -4511,10 +4595,13 @@
       <c r="F30" t="s">
         <v>695</v>
       </c>
-      <c r="G30" t="b">
+      <c r="G30">
         <v>0</v>
       </c>
-      <c r="H30" t="b">
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
         <v>0</v>
       </c>
       <c r="K30" s="5"/>
@@ -4577,10 +4664,13 @@
       <c r="F31" t="s">
         <v>696</v>
       </c>
-      <c r="G31" t="b">
+      <c r="G31">
         <v>0</v>
       </c>
-      <c r="H31" t="b">
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
         <v>0</v>
       </c>
       <c r="K31" s="5"/>
@@ -4643,10 +4733,13 @@
       <c r="F32" t="s">
         <v>697</v>
       </c>
-      <c r="G32" t="b">
+      <c r="G32">
         <v>0</v>
       </c>
-      <c r="H32" t="b">
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
         <v>0</v>
       </c>
       <c r="K32" s="5"/>
@@ -4709,11 +4802,14 @@
       <c r="F33" t="s">
         <v>698</v>
       </c>
-      <c r="G33" t="b">
+      <c r="G33">
         <v>1</v>
       </c>
-      <c r="H33" t="b">
+      <c r="H33">
         <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
       </c>
       <c r="K33" s="5"/>
       <c r="L33" s="6"/>
@@ -4775,10 +4871,13 @@
       <c r="F34" t="s">
         <v>699</v>
       </c>
-      <c r="G34" t="b">
+      <c r="G34">
         <v>0</v>
       </c>
-      <c r="H34" t="b">
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
         <v>0</v>
       </c>
       <c r="K34" s="5"/>
@@ -4841,10 +4940,13 @@
       <c r="F35" t="s">
         <v>700</v>
       </c>
-      <c r="G35" t="b">
+      <c r="G35">
         <v>0</v>
       </c>
-      <c r="H35" t="b">
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
         <v>0</v>
       </c>
       <c r="K35" s="5"/>
@@ -4907,10 +5009,13 @@
       <c r="F36" t="s">
         <v>701</v>
       </c>
-      <c r="G36" t="b">
+      <c r="G36">
         <v>0</v>
       </c>
-      <c r="H36" t="b">
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
         <v>0</v>
       </c>
       <c r="K36" s="5"/>
@@ -4973,10 +5078,13 @@
       <c r="F37" t="s">
         <v>702</v>
       </c>
-      <c r="G37" t="b">
+      <c r="G37">
         <v>0</v>
       </c>
-      <c r="H37" t="b">
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
         <v>0</v>
       </c>
       <c r="K37" s="5"/>
@@ -5039,11 +5147,14 @@
       <c r="F38" t="s">
         <v>703</v>
       </c>
-      <c r="G38" t="b">
+      <c r="G38">
         <v>0</v>
       </c>
-      <c r="H38" t="b">
+      <c r="H38">
         <v>1</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="6"/>
@@ -5105,10 +5216,13 @@
       <c r="F39" t="s">
         <v>704</v>
       </c>
-      <c r="G39" t="b">
+      <c r="G39">
         <v>0</v>
       </c>
-      <c r="H39" t="b">
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
         <v>0</v>
       </c>
       <c r="K39" s="5"/>
@@ -5171,10 +5285,13 @@
       <c r="F40" t="s">
         <v>705</v>
       </c>
-      <c r="G40" t="b">
+      <c r="G40">
         <v>0</v>
       </c>
-      <c r="H40" t="b">
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
         <v>0</v>
       </c>
       <c r="K40" s="5"/>
@@ -5237,11 +5354,14 @@
       <c r="F41" t="s">
         <v>706</v>
       </c>
-      <c r="G41" t="b">
+      <c r="G41">
         <v>0</v>
       </c>
-      <c r="H41" t="b">
+      <c r="H41">
         <v>1</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
       </c>
       <c r="K41" s="5"/>
       <c r="L41" s="6"/>
@@ -5303,10 +5423,13 @@
       <c r="F42" t="s">
         <v>707</v>
       </c>
-      <c r="G42" t="b">
+      <c r="G42">
         <v>0</v>
       </c>
-      <c r="H42" t="b">
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
         <v>0</v>
       </c>
       <c r="K42" s="5"/>
@@ -5369,11 +5492,14 @@
       <c r="F43" t="s">
         <v>708</v>
       </c>
-      <c r="G43" t="b">
+      <c r="G43">
         <v>1</v>
       </c>
-      <c r="H43" t="b">
+      <c r="H43">
         <v>1</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="6"/>
@@ -5435,10 +5561,13 @@
       <c r="F44" t="s">
         <v>709</v>
       </c>
-      <c r="G44" t="b">
+      <c r="G44">
         <v>0</v>
       </c>
-      <c r="H44" t="b">
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
         <v>0</v>
       </c>
       <c r="K44" s="5"/>
@@ -5501,10 +5630,13 @@
       <c r="F45" t="s">
         <v>710</v>
       </c>
-      <c r="G45" t="b">
+      <c r="G45">
         <v>0</v>
       </c>
-      <c r="H45" t="b">
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
         <v>0</v>
       </c>
       <c r="K45" s="5"/>
@@ -5567,11 +5699,14 @@
       <c r="F46" t="s">
         <v>711</v>
       </c>
-      <c r="G46" t="b">
+      <c r="G46">
         <v>0</v>
       </c>
-      <c r="H46" t="b">
+      <c r="H46">
         <v>1</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="6"/>
@@ -5633,10 +5768,13 @@
       <c r="F47" t="s">
         <v>712</v>
       </c>
-      <c r="G47" t="b">
+      <c r="G47">
         <v>0</v>
       </c>
-      <c r="H47" t="b">
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
         <v>0</v>
       </c>
       <c r="K47" s="5"/>
@@ -5699,10 +5837,13 @@
       <c r="F48" t="s">
         <v>713</v>
       </c>
-      <c r="G48" t="b">
+      <c r="G48">
         <v>0</v>
       </c>
-      <c r="H48" t="b">
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
         <v>0</v>
       </c>
       <c r="K48" s="5"/>
@@ -5765,10 +5906,13 @@
       <c r="F49" t="s">
         <v>714</v>
       </c>
-      <c r="G49" t="b">
+      <c r="G49">
         <v>0</v>
       </c>
-      <c r="H49" t="b">
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
         <v>0</v>
       </c>
       <c r="K49" s="5"/>
@@ -5831,10 +5975,13 @@
       <c r="F50" t="s">
         <v>715</v>
       </c>
-      <c r="G50" t="b">
+      <c r="G50">
         <v>0</v>
       </c>
-      <c r="H50" t="b">
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
         <v>0</v>
       </c>
       <c r="K50" s="5"/>
@@ -5897,10 +6044,13 @@
       <c r="F51" t="s">
         <v>716</v>
       </c>
-      <c r="G51" t="b">
+      <c r="G51">
         <v>0</v>
       </c>
-      <c r="H51" t="b">
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
         <v>0</v>
       </c>
       <c r="K51" s="5"/>
@@ -5963,10 +6113,13 @@
       <c r="F52" t="s">
         <v>717</v>
       </c>
-      <c r="G52" t="b">
+      <c r="G52">
         <v>0</v>
       </c>
-      <c r="H52" t="b">
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
         <v>0</v>
       </c>
       <c r="K52" s="5"/>
@@ -10062,10 +10215,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:H1"/>
     <mergeCell ref="AN1:BC1"/>
     <mergeCell ref="A55:P55"/>
     <mergeCell ref="A159:L159"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10708,7 +10861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B78DEF-5A20-47DD-A1BF-E039EC331573}">
   <dimension ref="A1:X102"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
@@ -15818,7 +15971,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15853,7 +16006,7 @@
       <c r="B3" t="s">
         <v>636</v>
       </c>
-      <c r="C3" t="b">
+      <c r="C3">
         <v>1</v>
       </c>
     </row>
@@ -15864,7 +16017,7 @@
       <c r="B4" t="s">
         <v>637</v>
       </c>
-      <c r="C4" t="b">
+      <c r="C4">
         <v>0</v>
       </c>
     </row>
@@ -15875,7 +16028,7 @@
       <c r="B5" t="s">
         <v>638</v>
       </c>
-      <c r="C5" t="b">
+      <c r="C5">
         <v>1</v>
       </c>
     </row>
@@ -15886,7 +16039,7 @@
       <c r="B6" t="s">
         <v>636</v>
       </c>
-      <c r="C6" t="b">
+      <c r="C6">
         <v>0</v>
       </c>
     </row>
@@ -15897,7 +16050,7 @@
       <c r="B7" t="s">
         <v>637</v>
       </c>
-      <c r="C7" t="b">
+      <c r="C7">
         <v>1</v>
       </c>
     </row>
@@ -15908,7 +16061,7 @@
       <c r="B8" t="s">
         <v>638</v>
       </c>
-      <c r="C8" t="b">
+      <c r="C8">
         <v>1</v>
       </c>
     </row>
@@ -15919,7 +16072,7 @@
       <c r="B9" t="s">
         <v>636</v>
       </c>
-      <c r="C9" t="b">
+      <c r="C9">
         <v>0</v>
       </c>
     </row>
@@ -15930,7 +16083,7 @@
       <c r="B10" t="s">
         <v>637</v>
       </c>
-      <c r="C10" t="b">
+      <c r="C10">
         <v>1</v>
       </c>
     </row>
@@ -15941,7 +16094,7 @@
       <c r="B11" t="s">
         <v>638</v>
       </c>
-      <c r="C11" t="b">
+      <c r="C11">
         <v>1</v>
       </c>
     </row>
@@ -15952,7 +16105,7 @@
       <c r="B12" t="s">
         <v>636</v>
       </c>
-      <c r="C12" t="b">
+      <c r="C12">
         <v>1</v>
       </c>
     </row>
@@ -15963,7 +16116,7 @@
       <c r="B13" t="s">
         <v>637</v>
       </c>
-      <c r="C13" t="b">
+      <c r="C13">
         <v>1</v>
       </c>
     </row>
@@ -15974,7 +16127,7 @@
       <c r="B14" t="s">
         <v>638</v>
       </c>
-      <c r="C14" t="b">
+      <c r="C14">
         <v>1</v>
       </c>
     </row>
@@ -15985,7 +16138,7 @@
       <c r="B15" t="s">
         <v>636</v>
       </c>
-      <c r="C15" t="b">
+      <c r="C15">
         <v>0</v>
       </c>
     </row>
@@ -15996,7 +16149,7 @@
       <c r="B16" t="s">
         <v>637</v>
       </c>
-      <c r="C16" t="b">
+      <c r="C16">
         <v>1</v>
       </c>
     </row>
@@ -16007,7 +16160,7 @@
       <c r="B17" t="s">
         <v>638</v>
       </c>
-      <c r="C17" t="b">
+      <c r="C17">
         <v>1</v>
       </c>
     </row>
@@ -16018,7 +16171,7 @@
       <c r="B18" t="s">
         <v>636</v>
       </c>
-      <c r="C18" t="b">
+      <c r="C18">
         <v>1</v>
       </c>
     </row>
@@ -16029,7 +16182,7 @@
       <c r="B19" t="s">
         <v>637</v>
       </c>
-      <c r="C19" t="b">
+      <c r="C19">
         <v>0</v>
       </c>
     </row>
@@ -16040,7 +16193,7 @@
       <c r="B20" t="s">
         <v>638</v>
       </c>
-      <c r="C20" t="b">
+      <c r="C20">
         <v>1</v>
       </c>
     </row>
@@ -16051,7 +16204,7 @@
       <c r="B21" t="s">
         <v>636</v>
       </c>
-      <c r="C21" t="b">
+      <c r="C21">
         <v>1</v>
       </c>
     </row>
@@ -16062,7 +16215,7 @@
       <c r="B22" t="s">
         <v>637</v>
       </c>
-      <c r="C22" t="b">
+      <c r="C22">
         <v>1</v>
       </c>
     </row>
@@ -16073,7 +16226,7 @@
       <c r="B23" t="s">
         <v>638</v>
       </c>
-      <c r="C23" t="b">
+      <c r="C23">
         <v>0</v>
       </c>
     </row>
@@ -16084,7 +16237,7 @@
       <c r="B24" t="s">
         <v>636</v>
       </c>
-      <c r="C24" t="b">
+      <c r="C24">
         <v>0</v>
       </c>
     </row>
@@ -16095,7 +16248,7 @@
       <c r="B25" t="s">
         <v>637</v>
       </c>
-      <c r="C25" t="b">
+      <c r="C25">
         <v>0</v>
       </c>
     </row>
@@ -16106,7 +16259,7 @@
       <c r="B26" t="s">
         <v>638</v>
       </c>
-      <c r="C26" t="b">
+      <c r="C26">
         <v>1</v>
       </c>
     </row>
@@ -16117,7 +16270,7 @@
       <c r="B27" t="s">
         <v>636</v>
       </c>
-      <c r="C27" t="b">
+      <c r="C27">
         <v>0</v>
       </c>
     </row>
@@ -16128,7 +16281,7 @@
       <c r="B28" t="s">
         <v>637</v>
       </c>
-      <c r="C28" t="b">
+      <c r="C28">
         <v>1</v>
       </c>
     </row>
@@ -16139,7 +16292,7 @@
       <c r="B29" t="s">
         <v>638</v>
       </c>
-      <c r="C29" t="b">
+      <c r="C29">
         <v>0</v>
       </c>
     </row>
@@ -16150,7 +16303,7 @@
       <c r="B30" t="s">
         <v>636</v>
       </c>
-      <c r="C30" t="b">
+      <c r="C30">
         <v>1</v>
       </c>
     </row>
@@ -16161,7 +16314,7 @@
       <c r="B31" t="s">
         <v>637</v>
       </c>
-      <c r="C31" t="b">
+      <c r="C31">
         <v>1</v>
       </c>
     </row>
@@ -16172,7 +16325,7 @@
       <c r="B32" t="s">
         <v>638</v>
       </c>
-      <c r="C32" t="b">
+      <c r="C32">
         <v>1</v>
       </c>
     </row>
@@ -16183,7 +16336,7 @@
       <c r="B33" t="s">
         <v>636</v>
       </c>
-      <c r="C33" t="b">
+      <c r="C33">
         <v>0</v>
       </c>
     </row>
@@ -16194,7 +16347,7 @@
       <c r="B34" t="s">
         <v>637</v>
       </c>
-      <c r="C34" t="b">
+      <c r="C34">
         <v>0</v>
       </c>
     </row>
@@ -16205,7 +16358,7 @@
       <c r="B35" t="s">
         <v>638</v>
       </c>
-      <c r="C35" t="b">
+      <c r="C35">
         <v>0</v>
       </c>
     </row>
@@ -16216,7 +16369,7 @@
       <c r="B36" t="s">
         <v>636</v>
       </c>
-      <c r="C36" t="b">
+      <c r="C36">
         <v>1</v>
       </c>
     </row>
@@ -16227,7 +16380,7 @@
       <c r="B37" t="s">
         <v>637</v>
       </c>
-      <c r="C37" t="b">
+      <c r="C37">
         <v>1</v>
       </c>
     </row>
@@ -16238,7 +16391,7 @@
       <c r="B38" t="s">
         <v>638</v>
       </c>
-      <c r="C38" t="b">
+      <c r="C38">
         <v>0</v>
       </c>
     </row>
@@ -16249,7 +16402,7 @@
       <c r="B39" t="s">
         <v>636</v>
       </c>
-      <c r="C39" t="b">
+      <c r="C39">
         <v>1</v>
       </c>
     </row>
@@ -16260,7 +16413,7 @@
       <c r="B40" t="s">
         <v>637</v>
       </c>
-      <c r="C40" t="b">
+      <c r="C40">
         <v>0</v>
       </c>
     </row>
@@ -16271,7 +16424,7 @@
       <c r="B41" t="s">
         <v>638</v>
       </c>
-      <c r="C41" t="b">
+      <c r="C41">
         <v>0</v>
       </c>
     </row>
@@ -16282,7 +16435,7 @@
       <c r="B42" t="s">
         <v>636</v>
       </c>
-      <c r="C42" t="b">
+      <c r="C42">
         <v>0</v>
       </c>
     </row>
@@ -16293,7 +16446,7 @@
       <c r="B43" t="s">
         <v>637</v>
       </c>
-      <c r="C43" t="b">
+      <c r="C43">
         <v>1</v>
       </c>
     </row>
@@ -16304,7 +16457,7 @@
       <c r="B44" t="s">
         <v>638</v>
       </c>
-      <c r="C44" t="b">
+      <c r="C44">
         <v>1</v>
       </c>
     </row>
@@ -16315,7 +16468,7 @@
       <c r="B45" t="s">
         <v>636</v>
       </c>
-      <c r="C45" t="b">
+      <c r="C45">
         <v>1</v>
       </c>
     </row>
@@ -16326,7 +16479,7 @@
       <c r="B46" t="s">
         <v>637</v>
       </c>
-      <c r="C46" t="b">
+      <c r="C46">
         <v>1</v>
       </c>
     </row>
@@ -16337,7 +16490,7 @@
       <c r="B47" t="s">
         <v>638</v>
       </c>
-      <c r="C47" t="b">
+      <c r="C47">
         <v>1</v>
       </c>
     </row>
@@ -16348,7 +16501,7 @@
       <c r="B48" t="s">
         <v>636</v>
       </c>
-      <c r="C48" t="b">
+      <c r="C48">
         <v>1</v>
       </c>
     </row>
@@ -16359,7 +16512,7 @@
       <c r="B49" t="s">
         <v>637</v>
       </c>
-      <c r="C49" t="b">
+      <c r="C49">
         <v>1</v>
       </c>
     </row>
@@ -16370,7 +16523,7 @@
       <c r="B50" t="s">
         <v>638</v>
       </c>
-      <c r="C50" t="b">
+      <c r="C50">
         <v>0</v>
       </c>
     </row>
@@ -16381,7 +16534,7 @@
       <c r="B51" t="s">
         <v>636</v>
       </c>
-      <c r="C51" t="b">
+      <c r="C51">
         <v>1</v>
       </c>
     </row>
@@ -16392,7 +16545,7 @@
       <c r="B52" t="s">
         <v>637</v>
       </c>
-      <c r="C52" t="b">
+      <c r="C52">
         <v>0</v>
       </c>
     </row>
@@ -16408,8 +16561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453BF516-0E69-4C4C-8F9B-B3AE6048F2E1}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Flag data and csv files for quick inporting to the database
</commit_message>
<xml_diff>
--- a/Database Data.xlsx
+++ b/Database Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylwa\source\repos\CIS424_wi21_Med_Cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F316DE15-4202-419D-9870-04FFAF317DB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9DD3F4-4A25-4961-A069-484F05980675}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="720">
   <si>
     <t>User_ID</t>
   </si>
@@ -2192,6 +2192,12 @@
   </si>
   <si>
     <t>b89o04dtcf6viujck</t>
+  </si>
+  <si>
+    <t>BByron2</t>
+  </si>
+  <si>
+    <t>EEllia2</t>
   </si>
 </sst>
 </file>
@@ -2252,7 +2258,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2265,11 +2271,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2278,7 +2283,18 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6F599AD3-6840-46F2-88F2-0E9C6FEC8D7E}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{099EC489-0DCF-455E-884E-0F2FAB91D948}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2557,7 +2573,7 @@
   <dimension ref="A1:BJ161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,22 +2637,22 @@
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="10"/>
+      <c r="BC1" s="10"/>
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
@@ -3063,7 +3079,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>718</v>
       </c>
       <c r="C8" t="s">
         <v>146</v>
@@ -5340,7 +5356,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>719</v>
       </c>
       <c r="C41" t="s">
         <v>179</v>
@@ -6248,22 +6264,22 @@
       <c r="BJ54" s="5"/>
     </row>
     <row r="55" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="12"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+      <c r="L55" s="10"/>
+      <c r="M55" s="10"/>
+      <c r="N55" s="10"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="10"/>
       <c r="Q55" s="5"/>
       <c r="R55" s="5"/>
       <c r="S55" s="5"/>
@@ -10169,18 +10185,18 @@
       <c r="T156" s="6"/>
     </row>
     <row r="159" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A159" s="12"/>
-      <c r="B159" s="12"/>
-      <c r="C159" s="12"/>
-      <c r="D159" s="12"/>
-      <c r="E159" s="12"/>
-      <c r="F159" s="12"/>
-      <c r="G159" s="12"/>
-      <c r="H159" s="12"/>
-      <c r="I159" s="12"/>
-      <c r="J159" s="12"/>
-      <c r="K159" s="12"/>
-      <c r="L159" s="12"/>
+      <c r="A159" s="10"/>
+      <c r="B159" s="10"/>
+      <c r="C159" s="10"/>
+      <c r="D159" s="10"/>
+      <c r="E159" s="10"/>
+      <c r="F159" s="10"/>
+      <c r="G159" s="10"/>
+      <c r="H159" s="10"/>
+      <c r="I159" s="10"/>
+      <c r="J159" s="10"/>
+      <c r="K159" s="10"/>
+      <c r="L159" s="10"/>
       <c r="M159" s="5"/>
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.25">
@@ -10221,6 +10237,9 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B3:B52">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10230,8 +10249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC7FE91-324E-4C19-B988-D44ECDAFF911}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10247,6 +10266,7 @@
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -10263,7 +10283,7 @@
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
-      <c r="L1" s="10"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -10299,6 +10319,9 @@
       <c r="K2" t="s">
         <v>470</v>
       </c>
+      <c r="L2" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -10334,6 +10357,9 @@
       <c r="K3">
         <v>48604</v>
       </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -10369,6 +10395,9 @@
       <c r="K4">
         <v>48601</v>
       </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -10404,6 +10433,9 @@
       <c r="K5">
         <v>48601</v>
       </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -10439,6 +10471,9 @@
       <c r="K6">
         <v>48707</v>
       </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -10474,6 +10509,9 @@
       <c r="K7">
         <v>48604</v>
       </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -10509,6 +10547,9 @@
       <c r="K8">
         <v>48601</v>
       </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -10544,6 +10585,9 @@
       <c r="K9">
         <v>48707</v>
       </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -10579,6 +10623,9 @@
       <c r="K10">
         <v>48601</v>
       </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -10614,6 +10661,9 @@
       <c r="K11">
         <v>48604</v>
       </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -10649,6 +10699,9 @@
       <c r="K12">
         <v>48601</v>
       </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -10684,6 +10737,9 @@
       <c r="K13">
         <v>48604</v>
       </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -10719,6 +10775,9 @@
       <c r="K14">
         <v>48707</v>
       </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -10754,6 +10813,9 @@
       <c r="K15">
         <v>48707</v>
       </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -10789,8 +10851,11 @@
       <c r="K16">
         <v>48601</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -10824,17 +10889,20 @@
       <c r="K17">
         <v>48601</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.25">
@@ -10851,7 +10919,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10862,7 +10930,7 @@
   <dimension ref="A1:X102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J98" sqref="J98"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10883,6 +10951,7 @@
     <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10905,6 +10974,7 @@
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
       <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -10955,6 +11025,9 @@
       <c r="P2" t="s">
         <v>213</v>
       </c>
+      <c r="Q2" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -11005,6 +11078,9 @@
       <c r="P3">
         <v>12</v>
       </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
       <c r="U3" s="9"/>
       <c r="X3" s="2"/>
     </row>
@@ -11057,6 +11133,9 @@
       <c r="P4">
         <v>1</v>
       </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -11107,6 +11186,9 @@
       <c r="P5">
         <v>12</v>
       </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -11157,6 +11239,9 @@
       <c r="P6">
         <v>15</v>
       </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -11207,6 +11292,9 @@
       <c r="P7">
         <v>4</v>
       </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -11257,6 +11345,9 @@
       <c r="P8">
         <v>11</v>
       </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -11307,6 +11398,9 @@
       <c r="P9">
         <v>11</v>
       </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -11357,6 +11451,9 @@
       <c r="P10">
         <v>2</v>
       </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -11407,6 +11504,9 @@
       <c r="P11">
         <v>11</v>
       </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -11457,6 +11557,9 @@
       <c r="P12">
         <v>11</v>
       </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -11507,6 +11610,9 @@
       <c r="P13">
         <v>13</v>
       </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -11557,6 +11663,9 @@
       <c r="P14">
         <v>5</v>
       </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -11607,6 +11716,9 @@
       <c r="P15">
         <v>3</v>
       </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -11657,8 +11769,11 @@
       <c r="P16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -11707,8 +11822,11 @@
       <c r="P17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -11757,8 +11875,11 @@
       <c r="P18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -11807,8 +11928,11 @@
       <c r="P19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -11857,8 +11981,11 @@
       <c r="P20">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -11907,8 +12034,11 @@
       <c r="P21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -11957,8 +12087,11 @@
       <c r="P22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -12007,8 +12140,11 @@
       <c r="P23">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -12057,8 +12193,11 @@
       <c r="P24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -12107,8 +12246,11 @@
       <c r="P25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -12157,8 +12299,11 @@
       <c r="P26">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -12207,8 +12352,11 @@
       <c r="P27">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -12257,8 +12405,11 @@
       <c r="P28">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -12307,8 +12458,11 @@
       <c r="P29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -12357,8 +12511,11 @@
       <c r="P30">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -12407,8 +12564,11 @@
       <c r="P31">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -12457,8 +12617,11 @@
       <c r="P32">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -12507,8 +12670,11 @@
       <c r="P33">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -12557,8 +12723,11 @@
       <c r="P34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -12607,8 +12776,11 @@
       <c r="P35">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -12657,8 +12829,11 @@
       <c r="P36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -12707,8 +12882,11 @@
       <c r="P37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -12757,8 +12935,11 @@
       <c r="P38">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -12807,8 +12988,11 @@
       <c r="P39">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -12857,8 +13041,11 @@
       <c r="P40">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -12907,8 +13094,11 @@
       <c r="P41">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -12957,8 +13147,11 @@
       <c r="P42">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -13007,8 +13200,11 @@
       <c r="P43">
         <v>11</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -13057,8 +13253,11 @@
       <c r="P44">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -13107,8 +13306,11 @@
       <c r="P45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -13157,8 +13359,11 @@
       <c r="P46">
         <v>15</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -13207,8 +13412,11 @@
       <c r="P47">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -13257,8 +13465,11 @@
       <c r="P48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -13307,8 +13518,11 @@
       <c r="P49">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -13357,8 +13571,11 @@
       <c r="P50">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -13407,8 +13624,11 @@
       <c r="P51">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -13457,8 +13677,11 @@
       <c r="P52">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -13507,8 +13730,11 @@
       <c r="P53">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -13557,8 +13783,11 @@
       <c r="P54">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -13607,8 +13836,11 @@
       <c r="P55">
         <v>14</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -13657,8 +13889,11 @@
       <c r="P56">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -13707,8 +13942,11 @@
       <c r="P57">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -13757,8 +13995,11 @@
       <c r="P58">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -13807,8 +14048,11 @@
       <c r="P59">
         <v>11</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -13857,8 +14101,11 @@
       <c r="P60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -13907,8 +14154,11 @@
       <c r="P61">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -13957,8 +14207,11 @@
       <c r="P62">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -14007,8 +14260,11 @@
       <c r="P63">
         <v>5</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -14057,8 +14313,11 @@
       <c r="P64">
         <v>12</v>
       </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -14107,8 +14366,11 @@
       <c r="P65">
         <v>11</v>
       </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -14157,8 +14419,11 @@
       <c r="P66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -14207,8 +14472,11 @@
       <c r="P67">
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -14257,8 +14525,11 @@
       <c r="P68">
         <v>8</v>
       </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -14307,8 +14578,11 @@
       <c r="P69">
         <v>13</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -14357,8 +14631,11 @@
       <c r="P70">
         <v>15</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -14407,8 +14684,11 @@
       <c r="P71">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -14457,8 +14737,11 @@
       <c r="P72">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -14507,8 +14790,11 @@
       <c r="P73">
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -14557,8 +14843,11 @@
       <c r="P74">
         <v>13</v>
       </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -14607,8 +14896,11 @@
       <c r="P75">
         <v>12</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -14657,8 +14949,11 @@
       <c r="P76">
         <v>13</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -14707,8 +15002,11 @@
       <c r="P77">
         <v>14</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -14757,8 +15055,11 @@
       <c r="P78">
         <v>7</v>
       </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -14807,8 +15108,11 @@
       <c r="P79">
         <v>7</v>
       </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -14857,8 +15161,11 @@
       <c r="P80">
         <v>15</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -14907,8 +15214,11 @@
       <c r="P81">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -14957,8 +15267,11 @@
       <c r="P82">
         <v>13</v>
       </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -15007,8 +15320,11 @@
       <c r="P83">
         <v>12</v>
       </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -15057,8 +15373,11 @@
       <c r="P84">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -15107,8 +15426,11 @@
       <c r="P85">
         <v>14</v>
       </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -15157,8 +15479,11 @@
       <c r="P86">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -15207,8 +15532,11 @@
       <c r="P87">
         <v>11</v>
       </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -15257,8 +15585,11 @@
       <c r="P88">
         <v>10</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -15307,8 +15638,11 @@
       <c r="P89">
         <v>6</v>
       </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -15357,8 +15691,11 @@
       <c r="P90">
         <v>12</v>
       </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -15407,8 +15744,11 @@
       <c r="P91">
         <v>12</v>
       </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -15457,8 +15797,11 @@
       <c r="P92">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -15507,8 +15850,11 @@
       <c r="P93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -15557,8 +15903,11 @@
       <c r="P94">
         <v>15</v>
       </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -15607,8 +15956,11 @@
       <c r="P95">
         <v>11</v>
       </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -15657,8 +16009,11 @@
       <c r="P96">
         <v>13</v>
       </c>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -15707,8 +16062,11 @@
       <c r="P97">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -15757,8 +16115,11 @@
       <c r="P98">
         <v>13</v>
       </c>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -15807,8 +16168,11 @@
       <c r="P99">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -15857,8 +16221,11 @@
       <c r="P100">
         <v>7</v>
       </c>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -15907,8 +16274,11 @@
       <c r="P101">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -15957,10 +16327,13 @@
       <c r="P102">
         <v>15</v>
       </c>
+      <c r="Q102">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16561,7 +16934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453BF516-0E69-4C4C-8F9B-B3AE6048F2E1}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added link to random name generator
</commit_message>
<xml_diff>
--- a/Database Data.xlsx
+++ b/Database Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylwa\source\repos\CIS424_wi21_Med_Cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD270BA-A71D-45B8-B0A5-71274824373A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45C331A-B5D6-4DFA-B2F5-BFA78C8424B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2412" uniqueCount="1102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="1104">
   <si>
     <t>User_ID</t>
   </si>
@@ -3366,6 +3366,12 @@
   </si>
   <si>
     <t>3761 Myrtle St</t>
+  </si>
+  <si>
+    <t>For names I use this site</t>
+  </si>
+  <si>
+    <t>http://www.randat.com/</t>
   </si>
 </sst>
 </file>
@@ -3459,32 +3465,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6F599AD3-6840-46F2-88F2-0E9C6FEC8D7E}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{099EC489-0DCF-455E-884E-0F2FAB91D948}"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4022,17 +4018,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
       <c r="K1" s="4" t="s">
         <v>549</v>
       </c>
@@ -4053,22 +4049,22 @@
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="14"/>
-      <c r="AQ1" s="14"/>
-      <c r="AR1" s="14"/>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AW1" s="14"/>
-      <c r="AX1" s="14"/>
-      <c r="AY1" s="14"/>
-      <c r="AZ1" s="14"/>
-      <c r="BA1" s="14"/>
-      <c r="BB1" s="14"/>
-      <c r="BC1" s="14"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="17"/>
+      <c r="AZ1" s="17"/>
+      <c r="BA1" s="17"/>
+      <c r="BB1" s="17"/>
+      <c r="BC1" s="17"/>
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
@@ -12816,18 +12812,18 @@
       <c r="T156" s="6"/>
     </row>
     <row r="159" spans="1:20">
-      <c r="A159" s="14"/>
-      <c r="B159" s="14"/>
-      <c r="C159" s="14"/>
-      <c r="D159" s="14"/>
-      <c r="E159" s="14"/>
-      <c r="F159" s="14"/>
-      <c r="G159" s="14"/>
-      <c r="H159" s="14"/>
-      <c r="I159" s="14"/>
-      <c r="J159" s="14"/>
-      <c r="K159" s="14"/>
-      <c r="L159" s="14"/>
+      <c r="A159" s="17"/>
+      <c r="B159" s="17"/>
+      <c r="C159" s="17"/>
+      <c r="D159" s="17"/>
+      <c r="E159" s="17"/>
+      <c r="F159" s="17"/>
+      <c r="G159" s="17"/>
+      <c r="H159" s="17"/>
+      <c r="I159" s="17"/>
+      <c r="J159" s="17"/>
+      <c r="K159" s="17"/>
+      <c r="L159" s="17"/>
       <c r="M159" s="5"/>
     </row>
     <row r="160" spans="1:20">
@@ -12868,10 +12864,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:B52">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12905,20 +12901,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>416</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
@@ -12972,7 +12968,7 @@
       <c r="L2" t="s">
         <v>433</v>
       </c>
-      <c r="O2" s="18"/>
+      <c r="O2" s="16"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
@@ -13016,7 +13012,7 @@
       <c r="I3" t="s">
         <v>711</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="15" t="s">
         <v>640</v>
       </c>
       <c r="K3" s="2">
@@ -13025,7 +13021,7 @@
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="O3" s="18"/>
+      <c r="O3" s="16"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
@@ -13069,7 +13065,7 @@
       <c r="I4" t="s">
         <v>723</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="15" t="s">
         <v>617</v>
       </c>
       <c r="K4" s="2">
@@ -13078,7 +13074,7 @@
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="O4" s="18"/>
+      <c r="O4" s="16"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
@@ -13122,7 +13118,7 @@
       <c r="I5" t="s">
         <v>699</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="15" t="s">
         <v>614</v>
       </c>
       <c r="K5" s="2">
@@ -13131,7 +13127,7 @@
       <c r="L5">
         <v>1</v>
       </c>
-      <c r="O5" s="18"/>
+      <c r="O5" s="16"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -13175,7 +13171,7 @@
       <c r="I6" t="s">
         <v>408</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="15" t="s">
         <v>637</v>
       </c>
       <c r="K6" s="2">
@@ -13184,7 +13180,7 @@
       <c r="L6">
         <v>1</v>
       </c>
-      <c r="O6" s="18"/>
+      <c r="O6" s="16"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
@@ -13228,7 +13224,7 @@
       <c r="I7" t="s">
         <v>735</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="15" t="s">
         <v>630</v>
       </c>
       <c r="K7" s="2">
@@ -13237,7 +13233,7 @@
       <c r="L7">
         <v>1</v>
       </c>
-      <c r="O7" s="18"/>
+      <c r="O7" s="16"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
@@ -13278,7 +13274,7 @@
       <c r="I8" t="s">
         <v>705</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="15" t="s">
         <v>622</v>
       </c>
       <c r="K8" s="2">
@@ -13287,7 +13283,7 @@
       <c r="L8">
         <v>1</v>
       </c>
-      <c r="O8" s="18"/>
+      <c r="O8" s="16"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
@@ -13331,7 +13327,7 @@
       <c r="I9" t="s">
         <v>725</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="15" t="s">
         <v>646</v>
       </c>
       <c r="K9" s="2">
@@ -13340,7 +13336,7 @@
       <c r="L9">
         <v>1</v>
       </c>
-      <c r="O9" s="18"/>
+      <c r="O9" s="16"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
@@ -13384,7 +13380,7 @@
       <c r="I10" t="s">
         <v>726</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="15" t="s">
         <v>621</v>
       </c>
       <c r="K10" s="2">
@@ -13393,7 +13389,7 @@
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="O10" s="18"/>
+      <c r="O10" s="16"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
@@ -13437,7 +13433,7 @@
       <c r="I11" t="s">
         <v>726</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="15" t="s">
         <v>622</v>
       </c>
       <c r="K11" s="2">
@@ -13446,7 +13442,7 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="O11" s="18"/>
+      <c r="O11" s="16"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
@@ -13490,7 +13486,7 @@
       <c r="I12" t="s">
         <v>699</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="15" t="s">
         <v>610</v>
       </c>
       <c r="K12" s="2">
@@ -13499,7 +13495,7 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="O12" s="18"/>
+      <c r="O12" s="16"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
@@ -13543,7 +13539,7 @@
       <c r="I13" t="s">
         <v>706</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="15" t="s">
         <v>630</v>
       </c>
       <c r="K13" s="2">
@@ -13552,7 +13548,7 @@
       <c r="L13">
         <v>1</v>
       </c>
-      <c r="O13" s="18"/>
+      <c r="O13" s="16"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
@@ -13596,7 +13592,7 @@
       <c r="I14" t="s">
         <v>699</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="15" t="s">
         <v>642</v>
       </c>
       <c r="K14" s="2">
@@ -13605,7 +13601,7 @@
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="O14" s="18"/>
+      <c r="O14" s="16"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
@@ -13649,7 +13645,7 @@
       <c r="I15" t="s">
         <v>725</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="15" t="s">
         <v>649</v>
       </c>
       <c r="K15" s="2">
@@ -13658,7 +13654,7 @@
       <c r="L15">
         <v>1</v>
       </c>
-      <c r="O15" s="18"/>
+      <c r="O15" s="16"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
@@ -13699,7 +13695,7 @@
       <c r="I16" t="s">
         <v>726</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="J16" s="15" t="s">
         <v>618</v>
       </c>
       <c r="K16" s="2">
@@ -13708,7 +13704,7 @@
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="O16" s="18"/>
+      <c r="O16" s="16"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
@@ -13752,7 +13748,7 @@
       <c r="I17" t="s">
         <v>704</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="15" t="s">
         <v>640</v>
       </c>
       <c r="K17" s="2">
@@ -13761,9 +13757,9 @@
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="O17" s="18"/>
+      <c r="O17" s="16"/>
       <c r="P17" s="5"/>
-      <c r="Q17" s="18"/>
+      <c r="Q17" s="16"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
@@ -13805,7 +13801,7 @@
       <c r="I18" t="s">
         <v>714</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="15" t="s">
         <v>608</v>
       </c>
       <c r="K18" s="2">
@@ -13814,7 +13810,7 @@
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="O18" s="18"/>
+      <c r="O18" s="16"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
@@ -13858,7 +13854,7 @@
       <c r="I19" t="s">
         <v>714</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J19" s="15" t="s">
         <v>647</v>
       </c>
       <c r="K19" s="2">
@@ -13867,7 +13863,7 @@
       <c r="L19">
         <v>1</v>
       </c>
-      <c r="O19" s="18"/>
+      <c r="O19" s="16"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
@@ -13911,7 +13907,7 @@
       <c r="I20" t="s">
         <v>710</v>
       </c>
-      <c r="J20" s="17" t="s">
+      <c r="J20" s="15" t="s">
         <v>627</v>
       </c>
       <c r="K20" s="2">
@@ -13920,7 +13916,7 @@
       <c r="L20">
         <v>0</v>
       </c>
-      <c r="O20" s="18"/>
+      <c r="O20" s="16"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
@@ -13964,7 +13960,7 @@
       <c r="I21" t="s">
         <v>708</v>
       </c>
-      <c r="J21" s="17" t="s">
+      <c r="J21" s="15" t="s">
         <v>612</v>
       </c>
       <c r="K21" s="2">
@@ -13973,7 +13969,7 @@
       <c r="L21">
         <v>1</v>
       </c>
-      <c r="O21" s="18"/>
+      <c r="O21" s="16"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
@@ -14017,7 +14013,7 @@
       <c r="I22" t="s">
         <v>408</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="J22" s="15" t="s">
         <v>619</v>
       </c>
       <c r="K22" s="2">
@@ -14026,7 +14022,7 @@
       <c r="L22">
         <v>1</v>
       </c>
-      <c r="O22" s="18"/>
+      <c r="O22" s="16"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
@@ -14070,7 +14066,7 @@
       <c r="I23" t="s">
         <v>701</v>
       </c>
-      <c r="J23" s="17" t="s">
+      <c r="J23" s="15" t="s">
         <v>620</v>
       </c>
       <c r="K23" s="2">
@@ -14079,7 +14075,7 @@
       <c r="L23">
         <v>1</v>
       </c>
-      <c r="O23" s="18"/>
+      <c r="O23" s="16"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
@@ -14123,7 +14119,7 @@
       <c r="I24" t="s">
         <v>732</v>
       </c>
-      <c r="J24" s="17" t="s">
+      <c r="J24" s="15" t="s">
         <v>628</v>
       </c>
       <c r="K24" s="2">
@@ -14132,7 +14128,7 @@
       <c r="L24">
         <v>0</v>
       </c>
-      <c r="O24" s="18"/>
+      <c r="O24" s="16"/>
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
@@ -14176,7 +14172,7 @@
       <c r="I25" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="17" t="s">
+      <c r="J25" s="15" t="s">
         <v>651</v>
       </c>
       <c r="K25" s="2">
@@ -14185,7 +14181,7 @@
       <c r="L25">
         <v>0</v>
       </c>
-      <c r="O25" s="18"/>
+      <c r="O25" s="16"/>
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
@@ -14229,7 +14225,7 @@
       <c r="I26" t="s">
         <v>732</v>
       </c>
-      <c r="J26" s="17" t="s">
+      <c r="J26" s="15" t="s">
         <v>620</v>
       </c>
       <c r="K26" s="2">
@@ -14238,7 +14234,7 @@
       <c r="L26">
         <v>1</v>
       </c>
-      <c r="O26" s="18"/>
+      <c r="O26" s="16"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
@@ -14282,7 +14278,7 @@
       <c r="I27" t="s">
         <v>705</v>
       </c>
-      <c r="J27" s="17" t="s">
+      <c r="J27" s="15" t="s">
         <v>640</v>
       </c>
       <c r="K27" s="2">
@@ -14291,7 +14287,7 @@
       <c r="L27">
         <v>0</v>
       </c>
-      <c r="O27" s="18"/>
+      <c r="O27" s="16"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
@@ -14332,7 +14328,7 @@
       <c r="I28" t="s">
         <v>731</v>
       </c>
-      <c r="J28" s="17" t="s">
+      <c r="J28" s="15" t="s">
         <v>645</v>
       </c>
       <c r="K28" s="2">
@@ -14341,7 +14337,7 @@
       <c r="L28">
         <v>0</v>
       </c>
-      <c r="O28" s="18"/>
+      <c r="O28" s="16"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
@@ -14385,7 +14381,7 @@
       <c r="I29" t="s">
         <v>741</v>
       </c>
-      <c r="J29" s="17" t="s">
+      <c r="J29" s="15" t="s">
         <v>650</v>
       </c>
       <c r="K29" s="2">
@@ -14394,7 +14390,7 @@
       <c r="L29">
         <v>1</v>
       </c>
-      <c r="O29" s="18"/>
+      <c r="O29" s="16"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
@@ -14438,7 +14434,7 @@
       <c r="I30" t="s">
         <v>740</v>
       </c>
-      <c r="J30" s="17" t="s">
+      <c r="J30" s="15" t="s">
         <v>620</v>
       </c>
       <c r="K30" s="2">
@@ -14447,7 +14443,7 @@
       <c r="L30">
         <v>0</v>
       </c>
-      <c r="O30" s="18"/>
+      <c r="O30" s="16"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
@@ -14491,7 +14487,7 @@
       <c r="I31" t="s">
         <v>14</v>
       </c>
-      <c r="J31" s="17" t="s">
+      <c r="J31" s="15" t="s">
         <v>651</v>
       </c>
       <c r="K31" s="2">
@@ -14500,7 +14496,7 @@
       <c r="L31">
         <v>1</v>
       </c>
-      <c r="O31" s="18"/>
+      <c r="O31" s="16"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
@@ -14544,7 +14540,7 @@
       <c r="I32" t="s">
         <v>728</v>
       </c>
-      <c r="J32" s="17" t="s">
+      <c r="J32" s="15" t="s">
         <v>613</v>
       </c>
       <c r="K32" s="2">
@@ -14553,7 +14549,7 @@
       <c r="L32">
         <v>0</v>
       </c>
-      <c r="O32" s="18"/>
+      <c r="O32" s="16"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
@@ -14597,7 +14593,7 @@
       <c r="I33" t="s">
         <v>694</v>
       </c>
-      <c r="J33" s="17" t="s">
+      <c r="J33" s="15" t="s">
         <v>640</v>
       </c>
       <c r="K33" s="2">
@@ -14606,7 +14602,7 @@
       <c r="L33">
         <v>0</v>
       </c>
-      <c r="O33" s="18"/>
+      <c r="O33" s="16"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
@@ -14650,7 +14646,7 @@
       <c r="I34" t="s">
         <v>694</v>
       </c>
-      <c r="J34" s="17" t="s">
+      <c r="J34" s="15" t="s">
         <v>650</v>
       </c>
       <c r="K34" s="2">
@@ -14659,7 +14655,7 @@
       <c r="L34">
         <v>0</v>
       </c>
-      <c r="O34" s="18"/>
+      <c r="O34" s="16"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
@@ -14703,7 +14699,7 @@
       <c r="I35" t="s">
         <v>711</v>
       </c>
-      <c r="J35" s="17" t="s">
+      <c r="J35" s="15" t="s">
         <v>643</v>
       </c>
       <c r="K35" s="2">
@@ -14712,7 +14708,7 @@
       <c r="L35">
         <v>1</v>
       </c>
-      <c r="O35" s="18"/>
+      <c r="O35" s="16"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
@@ -14756,7 +14752,7 @@
       <c r="I36" t="s">
         <v>723</v>
       </c>
-      <c r="J36" s="17" t="s">
+      <c r="J36" s="15" t="s">
         <v>632</v>
       </c>
       <c r="K36" s="2">
@@ -14765,7 +14761,7 @@
       <c r="L36">
         <v>1</v>
       </c>
-      <c r="O36" s="18"/>
+      <c r="O36" s="16"/>
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
@@ -14809,7 +14805,7 @@
       <c r="I37" t="s">
         <v>699</v>
       </c>
-      <c r="J37" s="17" t="s">
+      <c r="J37" s="15" t="s">
         <v>650</v>
       </c>
       <c r="K37" s="2">
@@ -14818,7 +14814,7 @@
       <c r="L37">
         <v>1</v>
       </c>
-      <c r="O37" s="18"/>
+      <c r="O37" s="16"/>
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
       <c r="R37" s="5"/>
@@ -14862,7 +14858,7 @@
       <c r="I38" t="s">
         <v>408</v>
       </c>
-      <c r="J38" s="17" t="s">
+      <c r="J38" s="15" t="s">
         <v>645</v>
       </c>
       <c r="K38" s="2">
@@ -14871,7 +14867,7 @@
       <c r="L38">
         <v>1</v>
       </c>
-      <c r="O38" s="18"/>
+      <c r="O38" s="16"/>
       <c r="P38" s="5"/>
       <c r="Q38" s="5"/>
       <c r="R38" s="5"/>
@@ -14915,7 +14911,7 @@
       <c r="I39" t="s">
         <v>735</v>
       </c>
-      <c r="J39" s="17" t="s">
+      <c r="J39" s="15" t="s">
         <v>604</v>
       </c>
       <c r="K39" s="2">
@@ -14924,7 +14920,7 @@
       <c r="L39">
         <v>1</v>
       </c>
-      <c r="O39" s="18"/>
+      <c r="O39" s="16"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
@@ -14968,7 +14964,7 @@
       <c r="I40" t="s">
         <v>705</v>
       </c>
-      <c r="J40" s="17" t="s">
+      <c r="J40" s="15" t="s">
         <v>647</v>
       </c>
       <c r="K40" s="2">
@@ -14977,7 +14973,7 @@
       <c r="L40">
         <v>0</v>
       </c>
-      <c r="O40" s="18"/>
+      <c r="O40" s="16"/>
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
       <c r="R40" s="5"/>
@@ -15021,7 +15017,7 @@
       <c r="I41" t="s">
         <v>725</v>
       </c>
-      <c r="J41" s="17" t="s">
+      <c r="J41" s="15" t="s">
         <v>645</v>
       </c>
       <c r="K41" s="2">
@@ -15030,7 +15026,7 @@
       <c r="L41">
         <v>0</v>
       </c>
-      <c r="O41" s="18"/>
+      <c r="O41" s="16"/>
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
@@ -15074,7 +15070,7 @@
       <c r="I42" t="s">
         <v>726</v>
       </c>
-      <c r="J42" s="17" t="s">
+      <c r="J42" s="15" t="s">
         <v>644</v>
       </c>
       <c r="K42" s="2">
@@ -15083,7 +15079,7 @@
       <c r="L42">
         <v>1</v>
       </c>
-      <c r="O42" s="18"/>
+      <c r="O42" s="16"/>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
@@ -15127,7 +15123,7 @@
       <c r="I43" t="s">
         <v>726</v>
       </c>
-      <c r="J43" s="17" t="s">
+      <c r="J43" s="15" t="s">
         <v>410</v>
       </c>
       <c r="K43" s="2">
@@ -15136,7 +15132,7 @@
       <c r="L43">
         <v>1</v>
       </c>
-      <c r="O43" s="18"/>
+      <c r="O43" s="16"/>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
       <c r="R43" s="5"/>
@@ -15180,7 +15176,7 @@
       <c r="I44" t="s">
         <v>699</v>
       </c>
-      <c r="J44" s="17" t="s">
+      <c r="J44" s="15" t="s">
         <v>616</v>
       </c>
       <c r="K44" s="2">
@@ -15189,7 +15185,7 @@
       <c r="L44">
         <v>1</v>
       </c>
-      <c r="O44" s="18"/>
+      <c r="O44" s="16"/>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
@@ -15233,7 +15229,7 @@
       <c r="I45" t="s">
         <v>706</v>
       </c>
-      <c r="J45" s="17" t="s">
+      <c r="J45" s="15" t="s">
         <v>647</v>
       </c>
       <c r="K45" s="2">
@@ -15242,7 +15238,7 @@
       <c r="L45">
         <v>1</v>
       </c>
-      <c r="O45" s="18"/>
+      <c r="O45" s="16"/>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
@@ -15286,7 +15282,7 @@
       <c r="I46" t="s">
         <v>699</v>
       </c>
-      <c r="J46" s="17" t="s">
+      <c r="J46" s="15" t="s">
         <v>605</v>
       </c>
       <c r="K46" s="2">
@@ -15295,7 +15291,7 @@
       <c r="L46">
         <v>0</v>
       </c>
-      <c r="O46" s="18"/>
+      <c r="O46" s="16"/>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
@@ -15339,7 +15335,7 @@
       <c r="I47" t="s">
         <v>725</v>
       </c>
-      <c r="J47" s="17" t="s">
+      <c r="J47" s="15" t="s">
         <v>639</v>
       </c>
       <c r="K47" s="2">
@@ -15348,7 +15344,7 @@
       <c r="L47">
         <v>1</v>
       </c>
-      <c r="O47" s="18"/>
+      <c r="O47" s="16"/>
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
       <c r="R47" s="5"/>
@@ -15392,7 +15388,7 @@
       <c r="I48" t="s">
         <v>726</v>
       </c>
-      <c r="J48" s="17" t="s">
+      <c r="J48" s="15" t="s">
         <v>610</v>
       </c>
       <c r="K48" s="2">
@@ -15401,7 +15397,7 @@
       <c r="L48">
         <v>0</v>
       </c>
-      <c r="O48" s="18"/>
+      <c r="O48" s="16"/>
       <c r="P48" s="5"/>
       <c r="Q48" s="5"/>
       <c r="R48" s="5"/>
@@ -15445,7 +15441,7 @@
       <c r="I49" t="s">
         <v>704</v>
       </c>
-      <c r="J49" s="17" t="s">
+      <c r="J49" s="15" t="s">
         <v>645</v>
       </c>
       <c r="K49" s="2">
@@ -15454,7 +15450,7 @@
       <c r="L49">
         <v>0</v>
       </c>
-      <c r="O49" s="18"/>
+      <c r="O49" s="16"/>
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
       <c r="R49" s="5"/>
@@ -15498,7 +15494,7 @@
       <c r="I50" t="s">
         <v>714</v>
       </c>
-      <c r="J50" s="17" t="s">
+      <c r="J50" s="15" t="s">
         <v>606</v>
       </c>
       <c r="K50" s="2">
@@ -15507,7 +15503,7 @@
       <c r="L50">
         <v>0</v>
       </c>
-      <c r="O50" s="18"/>
+      <c r="O50" s="16"/>
       <c r="P50" s="5"/>
       <c r="Q50" s="5"/>
       <c r="R50" s="5"/>
@@ -15551,7 +15547,7 @@
       <c r="I51" t="s">
         <v>709</v>
       </c>
-      <c r="J51" s="17" t="s">
+      <c r="J51" s="15" t="s">
         <v>633</v>
       </c>
       <c r="K51" s="2">
@@ -15560,7 +15556,7 @@
       <c r="L51">
         <v>0</v>
       </c>
-      <c r="O51" s="18"/>
+      <c r="O51" s="16"/>
       <c r="P51" s="5"/>
       <c r="Q51" s="5"/>
       <c r="R51" s="5"/>
@@ -15604,7 +15600,7 @@
       <c r="I52" t="s">
         <v>711</v>
       </c>
-      <c r="J52" s="17" t="s">
+      <c r="J52" s="15" t="s">
         <v>608</v>
       </c>
       <c r="K52" s="2">
@@ -15613,7 +15609,7 @@
       <c r="L52">
         <v>0</v>
       </c>
-      <c r="O52" s="18"/>
+      <c r="O52" s="16"/>
       <c r="P52" s="5"/>
       <c r="Q52" s="5"/>
       <c r="R52" s="5"/>
@@ -15654,7 +15650,7 @@
       <c r="I53" t="s">
         <v>707</v>
       </c>
-      <c r="J53" s="17" t="s">
+      <c r="J53" s="15" t="s">
         <v>613</v>
       </c>
       <c r="K53" s="2">
@@ -15663,7 +15659,7 @@
       <c r="L53">
         <v>0</v>
       </c>
-      <c r="O53" s="18"/>
+      <c r="O53" s="16"/>
       <c r="P53" s="5"/>
       <c r="Q53" s="5"/>
       <c r="R53" s="5"/>
@@ -15707,7 +15703,7 @@
       <c r="I54" t="s">
         <v>409</v>
       </c>
-      <c r="J54" s="17" t="s">
+      <c r="J54" s="15" t="s">
         <v>626</v>
       </c>
       <c r="K54" s="2">
@@ -15760,7 +15756,7 @@
       <c r="I55" t="s">
         <v>719</v>
       </c>
-      <c r="J55" s="17" t="s">
+      <c r="J55" s="15" t="s">
         <v>638</v>
       </c>
       <c r="K55" s="2">
@@ -15813,7 +15809,7 @@
       <c r="I56" t="s">
         <v>717</v>
       </c>
-      <c r="J56" s="17" t="s">
+      <c r="J56" s="15" t="s">
         <v>607</v>
       </c>
       <c r="K56" s="2">
@@ -15866,7 +15862,7 @@
       <c r="I57" t="s">
         <v>717</v>
       </c>
-      <c r="J57" s="17" t="s">
+      <c r="J57" s="15" t="s">
         <v>410</v>
       </c>
       <c r="K57" s="2">
@@ -15919,7 +15915,7 @@
       <c r="I58" t="s">
         <v>697</v>
       </c>
-      <c r="J58" s="17" t="s">
+      <c r="J58" s="15" t="s">
         <v>644</v>
       </c>
       <c r="K58" s="2">
@@ -15972,7 +15968,7 @@
       <c r="I59" t="s">
         <v>702</v>
       </c>
-      <c r="J59" s="17" t="s">
+      <c r="J59" s="15" t="s">
         <v>621</v>
       </c>
       <c r="K59" s="2">
@@ -16025,7 +16021,7 @@
       <c r="I60" t="s">
         <v>739</v>
       </c>
-      <c r="J60" s="17" t="s">
+      <c r="J60" s="15" t="s">
         <v>631</v>
       </c>
       <c r="K60" s="2">
@@ -16078,7 +16074,7 @@
       <c r="I61" t="s">
         <v>739</v>
       </c>
-      <c r="J61" s="17" t="s">
+      <c r="J61" s="15" t="s">
         <v>621</v>
       </c>
       <c r="K61" s="2">
@@ -16116,7 +16112,7 @@
       <c r="I62" t="s">
         <v>719</v>
       </c>
-      <c r="J62" s="17" t="s">
+      <c r="J62" s="15" t="s">
         <v>632</v>
       </c>
       <c r="K62" s="2">
@@ -16154,7 +16150,7 @@
       <c r="I63" t="s">
         <v>724</v>
       </c>
-      <c r="J63" s="17" t="s">
+      <c r="J63" s="15" t="s">
         <v>638</v>
       </c>
       <c r="K63" s="2">
@@ -16192,7 +16188,7 @@
       <c r="I64" t="s">
         <v>703</v>
       </c>
-      <c r="J64" s="17" t="s">
+      <c r="J64" s="15" t="s">
         <v>640</v>
       </c>
       <c r="K64" s="2">
@@ -16230,7 +16226,7 @@
       <c r="I65" t="s">
         <v>703</v>
       </c>
-      <c r="J65" s="17" t="s">
+      <c r="J65" s="15" t="s">
         <v>616</v>
       </c>
       <c r="K65" s="2">
@@ -16268,7 +16264,7 @@
       <c r="I66" t="s">
         <v>730</v>
       </c>
-      <c r="J66" s="17" t="s">
+      <c r="J66" s="15" t="s">
         <v>646</v>
       </c>
       <c r="K66" s="2">
@@ -16306,7 +16302,7 @@
       <c r="I67" t="s">
         <v>409</v>
       </c>
-      <c r="J67" s="17" t="s">
+      <c r="J67" s="15" t="s">
         <v>645</v>
       </c>
       <c r="K67" s="2">
@@ -16344,7 +16340,7 @@
       <c r="I68" t="s">
         <v>693</v>
       </c>
-      <c r="J68" s="17" t="s">
+      <c r="J68" s="15" t="s">
         <v>622</v>
       </c>
       <c r="K68" s="2">
@@ -16379,7 +16375,7 @@
       <c r="I69" t="s">
         <v>732</v>
       </c>
-      <c r="J69" s="17" t="s">
+      <c r="J69" s="15" t="s">
         <v>614</v>
       </c>
       <c r="K69" s="2">
@@ -16417,7 +16413,7 @@
       <c r="I70" t="s">
         <v>691</v>
       </c>
-      <c r="J70" s="17" t="s">
+      <c r="J70" s="15" t="s">
         <v>625</v>
       </c>
       <c r="K70" s="2">
@@ -16455,7 +16451,7 @@
       <c r="I71" t="s">
         <v>728</v>
       </c>
-      <c r="J71" s="17" t="s">
+      <c r="J71" s="15" t="s">
         <v>629</v>
       </c>
       <c r="K71" s="2">
@@ -16493,7 +16489,7 @@
       <c r="I72" t="s">
         <v>724</v>
       </c>
-      <c r="J72" s="17" t="s">
+      <c r="J72" s="15" t="s">
         <v>642</v>
       </c>
       <c r="K72" s="2">
@@ -16531,7 +16527,7 @@
       <c r="I73" t="s">
         <v>700</v>
       </c>
-      <c r="J73" s="17" t="s">
+      <c r="J73" s="15" t="s">
         <v>614</v>
       </c>
       <c r="K73" s="2">
@@ -16569,7 +16565,7 @@
       <c r="I74" t="s">
         <v>727</v>
       </c>
-      <c r="J74" s="17" t="s">
+      <c r="J74" s="15" t="s">
         <v>628</v>
       </c>
       <c r="K74" s="2">
@@ -16607,7 +16603,7 @@
       <c r="I75" t="s">
         <v>737</v>
       </c>
-      <c r="J75" s="17" t="s">
+      <c r="J75" s="15" t="s">
         <v>651</v>
       </c>
       <c r="K75" s="2">
@@ -16645,7 +16641,7 @@
       <c r="I76" t="s">
         <v>720</v>
       </c>
-      <c r="J76" s="17" t="s">
+      <c r="J76" s="15" t="s">
         <v>603</v>
       </c>
       <c r="K76" s="2">
@@ -16683,7 +16679,7 @@
       <c r="I77" t="s">
         <v>719</v>
       </c>
-      <c r="J77" s="17" t="s">
+      <c r="J77" s="15" t="s">
         <v>621</v>
       </c>
       <c r="K77" s="2">
@@ -16721,7 +16717,7 @@
       <c r="I78" t="s">
         <v>692</v>
       </c>
-      <c r="J78" s="17" t="s">
+      <c r="J78" s="15" t="s">
         <v>625</v>
       </c>
       <c r="K78" s="2">
@@ -16759,7 +16755,7 @@
       <c r="I79" t="s">
         <v>718</v>
       </c>
-      <c r="J79" s="17" t="s">
+      <c r="J79" s="15" t="s">
         <v>636</v>
       </c>
       <c r="K79" s="2">
@@ -16797,7 +16793,7 @@
       <c r="I80" t="s">
         <v>692</v>
       </c>
-      <c r="J80" s="17" t="s">
+      <c r="J80" s="15" t="s">
         <v>619</v>
       </c>
       <c r="K80" s="2">
@@ -16835,7 +16831,7 @@
       <c r="I81" t="s">
         <v>715</v>
       </c>
-      <c r="J81" s="17" t="s">
+      <c r="J81" s="15" t="s">
         <v>634</v>
       </c>
       <c r="K81" s="2">
@@ -16873,7 +16869,7 @@
       <c r="I82" t="s">
         <v>702</v>
       </c>
-      <c r="J82" s="17" t="s">
+      <c r="J82" s="15" t="s">
         <v>621</v>
       </c>
       <c r="K82" s="2">
@@ -16911,7 +16907,7 @@
       <c r="I83" t="s">
         <v>727</v>
       </c>
-      <c r="J83" s="17" t="s">
+      <c r="J83" s="15" t="s">
         <v>606</v>
       </c>
       <c r="K83" s="2">
@@ -16946,7 +16942,7 @@
       <c r="I84" t="s">
         <v>693</v>
       </c>
-      <c r="J84" s="17" t="s">
+      <c r="J84" s="15" t="s">
         <v>617</v>
       </c>
       <c r="K84" s="2">
@@ -16984,7 +16980,7 @@
       <c r="I85" t="s">
         <v>737</v>
       </c>
-      <c r="J85" s="17" t="s">
+      <c r="J85" s="15" t="s">
         <v>623</v>
       </c>
       <c r="K85" s="2">
@@ -17022,7 +17018,7 @@
       <c r="I86" t="s">
         <v>408</v>
       </c>
-      <c r="J86" s="17" t="s">
+      <c r="J86" s="15" t="s">
         <v>644</v>
       </c>
       <c r="K86" s="2">
@@ -17060,7 +17056,7 @@
       <c r="I87" t="s">
         <v>742</v>
       </c>
-      <c r="J87" s="17" t="s">
+      <c r="J87" s="15" t="s">
         <v>621</v>
       </c>
       <c r="K87" s="2">
@@ -17098,7 +17094,7 @@
       <c r="I88" t="s">
         <v>691</v>
       </c>
-      <c r="J88" s="17" t="s">
+      <c r="J88" s="15" t="s">
         <v>607</v>
       </c>
       <c r="K88" s="2">
@@ -17136,7 +17132,7 @@
       <c r="I89" t="s">
         <v>709</v>
       </c>
-      <c r="J89" s="17" t="s">
+      <c r="J89" s="15" t="s">
         <v>609</v>
       </c>
       <c r="K89" s="2">
@@ -17174,7 +17170,7 @@
       <c r="I90" t="s">
         <v>409</v>
       </c>
-      <c r="J90" s="17" t="s">
+      <c r="J90" s="15" t="s">
         <v>648</v>
       </c>
       <c r="K90" s="2">
@@ -17212,7 +17208,7 @@
       <c r="I91" t="s">
         <v>715</v>
       </c>
-      <c r="J91" s="17" t="s">
+      <c r="J91" s="15" t="s">
         <v>603</v>
       </c>
       <c r="K91" s="2">
@@ -17250,7 +17246,7 @@
       <c r="I92" t="s">
         <v>731</v>
       </c>
-      <c r="J92" s="17" t="s">
+      <c r="J92" s="15" t="s">
         <v>630</v>
       </c>
       <c r="K92" s="2">
@@ -17285,7 +17281,7 @@
       <c r="I93" t="s">
         <v>701</v>
       </c>
-      <c r="J93" s="17" t="s">
+      <c r="J93" s="15" t="s">
         <v>638</v>
       </c>
       <c r="K93" s="2">
@@ -17323,7 +17319,7 @@
       <c r="I94" t="s">
         <v>408</v>
       </c>
-      <c r="J94" s="17" t="s">
+      <c r="J94" s="15" t="s">
         <v>621</v>
       </c>
       <c r="K94" s="2">
@@ -17361,7 +17357,7 @@
       <c r="I95" t="s">
         <v>711</v>
       </c>
-      <c r="J95" s="17" t="s">
+      <c r="J95" s="15" t="s">
         <v>651</v>
       </c>
       <c r="K95" s="2">
@@ -17399,7 +17395,7 @@
       <c r="I96" t="s">
         <v>696</v>
       </c>
-      <c r="J96" s="17" t="s">
+      <c r="J96" s="15" t="s">
         <v>630</v>
       </c>
       <c r="K96" s="2">
@@ -17437,7 +17433,7 @@
       <c r="I97" t="s">
         <v>731</v>
       </c>
-      <c r="J97" s="17" t="s">
+      <c r="J97" s="15" t="s">
         <v>609</v>
       </c>
       <c r="K97" s="2">
@@ -17475,7 +17471,7 @@
       <c r="I98" t="s">
         <v>713</v>
       </c>
-      <c r="J98" s="17" t="s">
+      <c r="J98" s="15" t="s">
         <v>611</v>
       </c>
       <c r="K98" s="2">
@@ -17513,7 +17509,7 @@
       <c r="I99" t="s">
         <v>731</v>
       </c>
-      <c r="J99" s="17" t="s">
+      <c r="J99" s="15" t="s">
         <v>608</v>
       </c>
       <c r="K99" s="2">
@@ -17551,7 +17547,7 @@
       <c r="I100" t="s">
         <v>729</v>
       </c>
-      <c r="J100" s="17" t="s">
+      <c r="J100" s="15" t="s">
         <v>614</v>
       </c>
       <c r="K100" s="2">
@@ -17589,7 +17585,7 @@
       <c r="I101" t="s">
         <v>698</v>
       </c>
-      <c r="J101" s="17" t="s">
+      <c r="J101" s="15" t="s">
         <v>627</v>
       </c>
       <c r="K101" s="2">
@@ -17627,7 +17623,7 @@
       <c r="I102" t="s">
         <v>735</v>
       </c>
-      <c r="J102" s="17" t="s">
+      <c r="J102" s="15" t="s">
         <v>626</v>
       </c>
       <c r="K102" s="2">
@@ -17677,25 +17673,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>411</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
       <c r="T1" s="5"/>
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
@@ -17767,7 +17763,7 @@
         <v>433</v>
       </c>
       <c r="T2" s="5"/>
-      <c r="U2" s="18"/>
+      <c r="U2" s="16"/>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
@@ -17837,7 +17833,7 @@
         <v>1</v>
       </c>
       <c r="T3" s="5"/>
-      <c r="U3" s="18"/>
+      <c r="U3" s="16"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
@@ -17907,7 +17903,7 @@
         <v>1</v>
       </c>
       <c r="T4" s="5"/>
-      <c r="U4" s="18"/>
+      <c r="U4" s="16"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
@@ -17977,7 +17973,7 @@
         <v>0</v>
       </c>
       <c r="T5" s="5"/>
-      <c r="U5" s="18"/>
+      <c r="U5" s="16"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
@@ -18047,7 +18043,7 @@
         <v>0</v>
       </c>
       <c r="T6" s="5"/>
-      <c r="U6" s="18"/>
+      <c r="U6" s="16"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
@@ -18117,7 +18113,7 @@
         <v>1</v>
       </c>
       <c r="T7" s="5"/>
-      <c r="U7" s="18"/>
+      <c r="U7" s="16"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
@@ -18187,7 +18183,7 @@
         <v>1</v>
       </c>
       <c r="T8" s="5"/>
-      <c r="U8" s="18"/>
+      <c r="U8" s="16"/>
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
@@ -18257,7 +18253,7 @@
         <v>0</v>
       </c>
       <c r="T9" s="5"/>
-      <c r="U9" s="18"/>
+      <c r="U9" s="16"/>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
@@ -18327,7 +18323,7 @@
         <v>0</v>
       </c>
       <c r="T10" s="5"/>
-      <c r="U10" s="18"/>
+      <c r="U10" s="16"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
@@ -18397,7 +18393,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="5"/>
-      <c r="U11" s="18"/>
+      <c r="U11" s="16"/>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
@@ -18467,7 +18463,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="5"/>
-      <c r="U12" s="18"/>
+      <c r="U12" s="16"/>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
@@ -18537,7 +18533,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="5"/>
-      <c r="U13" s="18"/>
+      <c r="U13" s="16"/>
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
@@ -18604,7 +18600,7 @@
         <v>1</v>
       </c>
       <c r="T14" s="5"/>
-      <c r="U14" s="18"/>
+      <c r="U14" s="16"/>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
@@ -18674,7 +18670,7 @@
         <v>1</v>
       </c>
       <c r="T15" s="5"/>
-      <c r="U15" s="18"/>
+      <c r="U15" s="16"/>
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
@@ -18744,7 +18740,7 @@
         <v>1</v>
       </c>
       <c r="T16" s="5"/>
-      <c r="U16" s="18"/>
+      <c r="U16" s="16"/>
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
@@ -18814,9 +18810,9 @@
         <v>0</v>
       </c>
       <c r="T17" s="5"/>
-      <c r="U17" s="18"/>
+      <c r="U17" s="16"/>
       <c r="V17" s="5"/>
-      <c r="W17" s="18"/>
+      <c r="W17" s="16"/>
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
@@ -18884,7 +18880,7 @@
         <v>1</v>
       </c>
       <c r="T18" s="5"/>
-      <c r="U18" s="18"/>
+      <c r="U18" s="16"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
@@ -18954,7 +18950,7 @@
         <v>1</v>
       </c>
       <c r="T19" s="5"/>
-      <c r="U19" s="18"/>
+      <c r="U19" s="16"/>
       <c r="V19" s="5"/>
       <c r="W19" s="5"/>
       <c r="X19" s="5"/>
@@ -19024,7 +19020,7 @@
         <v>1</v>
       </c>
       <c r="T20" s="5"/>
-      <c r="U20" s="18"/>
+      <c r="U20" s="16"/>
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
       <c r="X20" s="5"/>
@@ -19094,7 +19090,7 @@
         <v>1</v>
       </c>
       <c r="T21" s="5"/>
-      <c r="U21" s="18"/>
+      <c r="U21" s="16"/>
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
       <c r="X21" s="5"/>
@@ -19164,7 +19160,7 @@
         <v>1</v>
       </c>
       <c r="T22" s="5"/>
-      <c r="U22" s="18"/>
+      <c r="U22" s="16"/>
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
@@ -19234,7 +19230,7 @@
         <v>1</v>
       </c>
       <c r="T23" s="5"/>
-      <c r="U23" s="18"/>
+      <c r="U23" s="16"/>
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
       <c r="X23" s="5"/>
@@ -19301,7 +19297,7 @@
         <v>0</v>
       </c>
       <c r="T24" s="5"/>
-      <c r="U24" s="18"/>
+      <c r="U24" s="16"/>
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
@@ -19371,7 +19367,7 @@
         <v>1</v>
       </c>
       <c r="T25" s="5"/>
-      <c r="U25" s="18"/>
+      <c r="U25" s="16"/>
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
@@ -19441,7 +19437,7 @@
         <v>1</v>
       </c>
       <c r="T26" s="5"/>
-      <c r="U26" s="18"/>
+      <c r="U26" s="16"/>
       <c r="V26" s="5"/>
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
@@ -19511,7 +19507,7 @@
         <v>1</v>
       </c>
       <c r="T27" s="5"/>
-      <c r="U27" s="18"/>
+      <c r="U27" s="16"/>
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
       <c r="X27" s="5"/>
@@ -19581,7 +19577,7 @@
         <v>1</v>
       </c>
       <c r="T28" s="5"/>
-      <c r="U28" s="18"/>
+      <c r="U28" s="16"/>
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
       <c r="X28" s="5"/>
@@ -19651,7 +19647,7 @@
         <v>1</v>
       </c>
       <c r="T29" s="5"/>
-      <c r="U29" s="18"/>
+      <c r="U29" s="16"/>
       <c r="V29" s="5"/>
       <c r="W29" s="5"/>
       <c r="X29" s="5"/>
@@ -19721,7 +19717,7 @@
         <v>0</v>
       </c>
       <c r="T30" s="5"/>
-      <c r="U30" s="18"/>
+      <c r="U30" s="16"/>
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
@@ -19791,7 +19787,7 @@
         <v>1</v>
       </c>
       <c r="T31" s="5"/>
-      <c r="U31" s="18"/>
+      <c r="U31" s="16"/>
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
       <c r="X31" s="5"/>
@@ -19861,7 +19857,7 @@
         <v>1</v>
       </c>
       <c r="T32" s="5"/>
-      <c r="U32" s="18"/>
+      <c r="U32" s="16"/>
       <c r="V32" s="5"/>
       <c r="W32" s="5"/>
       <c r="X32" s="5"/>
@@ -19931,7 +19927,7 @@
         <v>0</v>
       </c>
       <c r="T33" s="5"/>
-      <c r="U33" s="18"/>
+      <c r="U33" s="16"/>
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
       <c r="X33" s="5"/>
@@ -20001,7 +19997,7 @@
         <v>1</v>
       </c>
       <c r="T34" s="5"/>
-      <c r="U34" s="18"/>
+      <c r="U34" s="16"/>
       <c r="V34" s="5"/>
       <c r="W34" s="5"/>
       <c r="X34" s="5"/>
@@ -20071,7 +20067,7 @@
         <v>0</v>
       </c>
       <c r="T35" s="5"/>
-      <c r="U35" s="18"/>
+      <c r="U35" s="16"/>
       <c r="V35" s="5"/>
       <c r="W35" s="5"/>
       <c r="X35" s="5"/>
@@ -20141,7 +20137,7 @@
         <v>0</v>
       </c>
       <c r="T36" s="5"/>
-      <c r="U36" s="18"/>
+      <c r="U36" s="16"/>
       <c r="V36" s="5"/>
       <c r="W36" s="5"/>
       <c r="X36" s="5"/>
@@ -20211,7 +20207,7 @@
         <v>0</v>
       </c>
       <c r="T37" s="5"/>
-      <c r="U37" s="18"/>
+      <c r="U37" s="16"/>
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
       <c r="X37" s="5"/>
@@ -20281,7 +20277,7 @@
         <v>0</v>
       </c>
       <c r="T38" s="5"/>
-      <c r="U38" s="18"/>
+      <c r="U38" s="16"/>
       <c r="V38" s="5"/>
       <c r="W38" s="5"/>
       <c r="X38" s="5"/>
@@ -20351,7 +20347,7 @@
         <v>0</v>
       </c>
       <c r="T39" s="5"/>
-      <c r="U39" s="18"/>
+      <c r="U39" s="16"/>
       <c r="V39" s="5"/>
       <c r="W39" s="5"/>
       <c r="X39" s="5"/>
@@ -20421,7 +20417,7 @@
         <v>0</v>
       </c>
       <c r="T40" s="5"/>
-      <c r="U40" s="18"/>
+      <c r="U40" s="16"/>
       <c r="V40" s="5"/>
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
@@ -20491,7 +20487,7 @@
         <v>0</v>
       </c>
       <c r="T41" s="5"/>
-      <c r="U41" s="18"/>
+      <c r="U41" s="16"/>
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
       <c r="X41" s="5"/>
@@ -20561,7 +20557,7 @@
         <v>0</v>
       </c>
       <c r="T42" s="5"/>
-      <c r="U42" s="18"/>
+      <c r="U42" s="16"/>
       <c r="V42" s="5"/>
       <c r="W42" s="5"/>
       <c r="X42" s="5"/>
@@ -20631,7 +20627,7 @@
         <v>1</v>
       </c>
       <c r="T43" s="5"/>
-      <c r="U43" s="18"/>
+      <c r="U43" s="16"/>
       <c r="V43" s="5"/>
       <c r="W43" s="5"/>
       <c r="X43" s="5"/>
@@ -20701,7 +20697,7 @@
         <v>0</v>
       </c>
       <c r="T44" s="5"/>
-      <c r="U44" s="18"/>
+      <c r="U44" s="16"/>
       <c r="V44" s="5"/>
       <c r="W44" s="5"/>
       <c r="X44" s="5"/>
@@ -20771,7 +20767,7 @@
         <v>0</v>
       </c>
       <c r="T45" s="5"/>
-      <c r="U45" s="18"/>
+      <c r="U45" s="16"/>
       <c r="V45" s="5"/>
       <c r="W45" s="5"/>
       <c r="X45" s="5"/>
@@ -20841,7 +20837,7 @@
         <v>0</v>
       </c>
       <c r="T46" s="5"/>
-      <c r="U46" s="18"/>
+      <c r="U46" s="16"/>
       <c r="V46" s="5"/>
       <c r="W46" s="5"/>
       <c r="X46" s="5"/>
@@ -20911,7 +20907,7 @@
         <v>0</v>
       </c>
       <c r="T47" s="5"/>
-      <c r="U47" s="18"/>
+      <c r="U47" s="16"/>
       <c r="V47" s="5"/>
       <c r="W47" s="5"/>
       <c r="X47" s="5"/>
@@ -20981,7 +20977,7 @@
         <v>0</v>
       </c>
       <c r="T48" s="5"/>
-      <c r="U48" s="18"/>
+      <c r="U48" s="16"/>
       <c r="V48" s="5"/>
       <c r="W48" s="5"/>
       <c r="X48" s="5"/>
@@ -21051,7 +21047,7 @@
         <v>1</v>
       </c>
       <c r="T49" s="5"/>
-      <c r="U49" s="18"/>
+      <c r="U49" s="16"/>
       <c r="V49" s="5"/>
       <c r="W49" s="5"/>
       <c r="X49" s="5"/>
@@ -21118,7 +21114,7 @@
         <v>1</v>
       </c>
       <c r="T50" s="5"/>
-      <c r="U50" s="18"/>
+      <c r="U50" s="16"/>
       <c r="V50" s="5"/>
       <c r="W50" s="5"/>
       <c r="X50" s="5"/>
@@ -21188,7 +21184,7 @@
         <v>0</v>
       </c>
       <c r="T51" s="5"/>
-      <c r="U51" s="18"/>
+      <c r="U51" s="16"/>
       <c r="V51" s="5"/>
       <c r="W51" s="5"/>
       <c r="X51" s="5"/>
@@ -21258,7 +21254,7 @@
         <v>0</v>
       </c>
       <c r="T52" s="5"/>
-      <c r="U52" s="18"/>
+      <c r="U52" s="16"/>
       <c r="V52" s="5"/>
       <c r="W52" s="5"/>
       <c r="X52" s="5"/>
@@ -21328,7 +21324,7 @@
         <v>1</v>
       </c>
       <c r="T53" s="5"/>
-      <c r="U53" s="18"/>
+      <c r="U53" s="16"/>
       <c r="V53" s="5"/>
       <c r="W53" s="5"/>
       <c r="X53" s="5"/>
@@ -24080,7 +24076,7 @@
     <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
@@ -24094,7 +24090,7 @@
   <dimension ref="A1:AB100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24116,71 +24112,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>652</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14" t="s">
         <v>747</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>653</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="F1" s="14"/>
+      <c r="G1" s="14" t="s">
         <v>689</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14" t="s">
         <v>690</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14" t="s">
         <v>746</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16" t="s">
+      <c r="N1" s="14"/>
+      <c r="O1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="14" t="s">
         <v>1040</v>
       </c>
       <c r="Q1" s="5"/>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="18" t="s">
         <v>602</v>
       </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
       <c r="AB1" s="11"/>
     </row>
     <row r="2" spans="1:28" ht="15.75">
-      <c r="A2" s="17" t="str" cm="1">
+      <c r="A2" s="15" t="str" cm="1">
         <f t="array" aca="1" ref="A2" ca="1">INDEX($A$4:$A$54,RANDBETWEEN(1,COUNTA($A$4:$A$54)),1)</f>
-        <v>MI</v>
+        <v>AR</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)</f>
-        <v>4215982967</v>
+        <v>5596614882</v>
       </c>
       <c r="E2" t="str">
         <f ca="1">RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)</f>
-        <v>38654</v>
+        <v>17782</v>
       </c>
       <c r="G2" t="str" cm="1">
         <f t="array" aca="1" ref="G2" ca="1">(INDEX($H$4:$H$6,RANDBETWEEN(1,COUNTA($H$4:$H$6)),1))&amp;" "&amp;(INDEX($G$4:$G$38,RANDBETWEEN(1,COUNTA($G$4:$G$38)),1))</f>
-        <v>83488 Appold Dr</v>
+        <v>6400 Borland Ct</v>
       </c>
       <c r="J2" t="str" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">INDEX($J$4:$J$6,RANDBETWEEN(1,COUNTA($J$4:$J$6)),1)</f>
-        <v>Diagnose</v>
+        <v>Advisor</v>
       </c>
       <c r="M2" t="str" cm="1">
         <f t="array" aca="1" ref="M2" ca="1">INDEX($M$4:$M$60,RANDBETWEEN(1,COUNTA($M$4:$M$60)),1)</f>
@@ -24188,26 +24184,26 @@
       </c>
       <c r="O2" t="str">
         <f ca="1">IF($R$3=16,$U$37,IF($R$3=17, $U$38,IF($R$3=18,$U$39,IF($R$3=19,$U$40,IF($R$3=20,$U$41,IF($R$3=21,$U$42,IF($R$3=22,$U$43,IF($R$3=23,$U$44,IF($R$3=24,$U$45,IF($R$3=25,$U$46,""))))))))))</f>
-        <v>%Zbd7H%I3NnOd1tgp</v>
+        <v>dX^17pvcimjzU$8*S</v>
       </c>
       <c r="P2" s="3">
         <f ca="1">RANDBETWEEN(DATE(1910,1,1),DATE(2021,2,5))</f>
-        <v>25591</v>
+        <v>32232</v>
       </c>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
-      <c r="U2" s="16" t="s">
+      <c r="U2" s="14" t="s">
         <v>748</v>
       </c>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
       <c r="AB2" s="5"/>
     </row>
     <row r="3" spans="1:28" ht="15.75">
-      <c r="A3" s="17"/>
+      <c r="A3" s="15"/>
       <c r="R3" s="6">
         <f ca="1">RANDBETWEEN(16,25)</f>
         <v>18</v>
@@ -24217,23 +24213,23 @@
       </c>
       <c r="T3" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T3" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>k</v>
+        <v>A</v>
       </c>
       <c r="U3" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T18)</f>
-        <v>kEm0c8qO5X4txhjI</v>
+        <v>AjlksJOlsSbtn1F2</v>
       </c>
       <c r="V3" s="5"/>
       <c r="W3" s="5" t="str">
         <f ca="1">IF(R3=16,U3,IF(R3=17, U4,IF(R3=18,U5,IF(R3=19,U6,IF(R3=20,U7,IF(R3=21,U8,IF(R3=22,U9,IF(R3=23,U10,IF(R3=24,U11,IF(R3=25,U12,""))))))))))</f>
-        <v>kEm0c8qO5X4txhjIJJ</v>
+        <v>AjlksJOlsSbtn1F2QI</v>
       </c>
       <c r="X3" s="5"/>
       <c r="Y3" s="6"/>
       <c r="AB3" s="5"/>
     </row>
     <row r="4" spans="1:28" ht="15.75">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>603</v>
       </c>
       <c r="G4" t="s">
@@ -24241,7 +24237,7 @@
       </c>
       <c r="H4" t="str">
         <f ca="1">RANDBETWEEN(1,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>9573</v>
+        <v>6400</v>
       </c>
       <c r="J4" t="s">
         <v>500</v>
@@ -24255,11 +24251,11 @@
       </c>
       <c r="T4" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T4" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>E</v>
+        <v>j</v>
       </c>
       <c r="U4" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T19)</f>
-        <v>kEm0c8qO5X4txhjIJ</v>
+        <v>AjlksJOlsSbtn1F2Q</v>
       </c>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
@@ -24268,7 +24264,7 @@
       <c r="AB4" s="5"/>
     </row>
     <row r="5" spans="1:28" ht="15.75">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="15" t="s">
         <v>604</v>
       </c>
       <c r="G5" t="s">
@@ -24276,7 +24272,7 @@
       </c>
       <c r="H5" t="str">
         <f ca="1">RANDBETWEEN(1,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>83488</v>
+        <v>83169</v>
       </c>
       <c r="J5" t="s">
         <v>499</v>
@@ -24290,11 +24286,11 @@
       </c>
       <c r="T5" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T5" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="U5" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T20)</f>
-        <v>kEm0c8qO5X4txhjIJJ</v>
+        <v>AjlksJOlsSbtn1F2QI</v>
       </c>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
@@ -24303,7 +24299,7 @@
       <c r="AB5" s="5"/>
     </row>
     <row r="6" spans="1:28" ht="15.75">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="15" t="s">
         <v>605</v>
       </c>
       <c r="G6" t="s">
@@ -24311,7 +24307,7 @@
       </c>
       <c r="H6" t="str">
         <f ca="1">RANDBETWEEN(1,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>268381</v>
+        <v>585432</v>
       </c>
       <c r="J6" t="s">
         <v>498</v>
@@ -24323,13 +24319,13 @@
       <c r="S6" s="5">
         <v>3</v>
       </c>
-      <c r="T6" s="5" cm="1">
+      <c r="T6" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T6" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>0</v>
+        <v>k</v>
       </c>
       <c r="U6" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T21)</f>
-        <v>kEm0c8qO5X4txhjIJJE</v>
+        <v>AjlksJOlsSbtn1F2QIX</v>
       </c>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
@@ -24338,7 +24334,7 @@
       <c r="AB6" s="5"/>
     </row>
     <row r="7" spans="1:28" ht="15.75">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="15" t="s">
         <v>606</v>
       </c>
       <c r="G7" t="s">
@@ -24353,11 +24349,11 @@
       </c>
       <c r="T7" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T7" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>c</v>
+        <v>s</v>
       </c>
       <c r="U7" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T22)</f>
-        <v>kEm0c8qO5X4txhjIJJEa</v>
+        <v>AjlksJOlsSbtn1F2QIXb</v>
       </c>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
@@ -24366,7 +24362,7 @@
       <c r="AB7" s="5"/>
     </row>
     <row r="8" spans="1:28" ht="15.75">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15" t="s">
         <v>607</v>
       </c>
       <c r="G8" t="s">
@@ -24379,13 +24375,13 @@
       <c r="S8" s="5">
         <v>5</v>
       </c>
-      <c r="T8" s="5" cm="1">
+      <c r="T8" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T8" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>8</v>
+        <v>J</v>
       </c>
       <c r="U8" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T23)</f>
-        <v>kEm0c8qO5X4txhjIJJEat</v>
+        <v>AjlksJOlsSbtn1F2QIXbL</v>
       </c>
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
@@ -24394,7 +24390,7 @@
       <c r="AB8" s="5"/>
     </row>
     <row r="9" spans="1:28" ht="15.75">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="15" t="s">
         <v>608</v>
       </c>
       <c r="G9" t="s">
@@ -24409,11 +24405,11 @@
       </c>
       <c r="T9" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T9" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>q</v>
+        <v>O</v>
       </c>
       <c r="U9" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T24)</f>
-        <v>kEm0c8qO5X4txhjIJJEata</v>
+        <v>AjlksJOlsSbtn1F2QIXbLu</v>
       </c>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
@@ -24422,7 +24418,7 @@
       <c r="AB9" s="5"/>
     </row>
     <row r="10" spans="1:28" ht="15.75">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="15" t="s">
         <v>609</v>
       </c>
       <c r="G10" t="s">
@@ -24437,11 +24433,11 @@
       </c>
       <c r="T10" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T10" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>O</v>
+        <v>l</v>
       </c>
       <c r="U10" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T25)</f>
-        <v>kEm0c8qO5X4txhjIJJEataC</v>
+        <v>AjlksJOlsSbtn1F2QIXbLuJ</v>
       </c>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
@@ -24450,7 +24446,7 @@
       <c r="AB10" s="5"/>
     </row>
     <row r="11" spans="1:28" ht="15.75">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="15" t="s">
         <v>610</v>
       </c>
       <c r="G11" t="s">
@@ -24463,13 +24459,13 @@
       <c r="S11" s="5">
         <v>8</v>
       </c>
-      <c r="T11" s="5" cm="1">
+      <c r="T11" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T11" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>5</v>
+        <v>s</v>
       </c>
       <c r="U11" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T26)</f>
-        <v>kEm0c8qO5X4txhjIJJEataCP</v>
+        <v>AjlksJOlsSbtn1F2QIXbLuJH</v>
       </c>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
@@ -24478,7 +24474,7 @@
       <c r="AB11" s="5"/>
     </row>
     <row r="12" spans="1:28" ht="15.75">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>611</v>
       </c>
       <c r="G12" t="s">
@@ -24493,11 +24489,11 @@
       </c>
       <c r="T12" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T12" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>X</v>
+        <v>S</v>
       </c>
       <c r="U12" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T27)</f>
-        <v>kEm0c8qO5X4txhjIJJEataCPT</v>
+        <v>AjlksJOlsSbtn1F2QIXbLuJHo</v>
       </c>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
@@ -24506,7 +24502,7 @@
       <c r="AB12" s="5"/>
     </row>
     <row r="13" spans="1:28" ht="15.75">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="15" t="s">
         <v>612</v>
       </c>
       <c r="G13" t="s">
@@ -24519,9 +24515,9 @@
       <c r="S13" s="5" t="s">
         <v>551</v>
       </c>
-      <c r="T13" s="5" cm="1">
+      <c r="T13" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T13" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>4</v>
+        <v>b</v>
       </c>
       <c r="U13" s="7"/>
       <c r="V13" s="5"/>
@@ -24531,7 +24527,7 @@
       <c r="AB13" s="5"/>
     </row>
     <row r="14" spans="1:28" ht="15.75">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="15" t="s">
         <v>613</v>
       </c>
       <c r="G14" t="s">
@@ -24556,7 +24552,7 @@
       <c r="AB14" s="5"/>
     </row>
     <row r="15" spans="1:28" ht="15.75">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="15" t="s">
         <v>614</v>
       </c>
       <c r="G15" t="s">
@@ -24571,7 +24567,7 @@
       </c>
       <c r="T15" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T15" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>x</v>
+        <v>n</v>
       </c>
       <c r="U15" s="7"/>
       <c r="V15" s="5"/>
@@ -24581,9 +24577,13 @@
       <c r="AB15" s="5"/>
     </row>
     <row r="16" spans="1:28" ht="15.75">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="15" t="s">
         <v>615</v>
       </c>
+      <c r="C16" s="18" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D16" s="18"/>
       <c r="G16" t="s">
         <v>657</v>
       </c>
@@ -24594,9 +24594,9 @@
       <c r="S16" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="T16" s="5" t="str" cm="1">
+      <c r="T16" s="5" cm="1">
         <f t="array" aca="1" ref="T16" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>h</v>
+        <v>1</v>
       </c>
       <c r="U16" s="7"/>
       <c r="V16" s="5"/>
@@ -24606,8 +24606,11 @@
       <c r="AB16" s="5"/>
     </row>
     <row r="17" spans="1:28" ht="15.75">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="15" t="s">
         <v>616</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1103</v>
       </c>
       <c r="G17" t="s">
         <v>658</v>
@@ -24621,7 +24624,7 @@
       </c>
       <c r="T17" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T17" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>j</v>
+        <v>F</v>
       </c>
       <c r="U17" s="7"/>
       <c r="V17" s="5"/>
@@ -24631,7 +24634,7 @@
       <c r="AB17" s="5"/>
     </row>
     <row r="18" spans="1:28" ht="15.75">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="15" t="s">
         <v>617</v>
       </c>
       <c r="G18" t="s">
@@ -24644,9 +24647,9 @@
       <c r="S18" s="5" t="s">
         <v>556</v>
       </c>
-      <c r="T18" s="5" t="str" cm="1">
+      <c r="T18" s="5" cm="1">
         <f t="array" aca="1" ref="T18" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>I</v>
+        <v>2</v>
       </c>
       <c r="U18" s="7"/>
       <c r="V18" s="5"/>
@@ -24656,7 +24659,7 @@
       <c r="AB18" s="5"/>
     </row>
     <row r="19" spans="1:28" ht="15.75">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="15" t="s">
         <v>618</v>
       </c>
       <c r="G19" t="s">
@@ -24671,7 +24674,7 @@
       </c>
       <c r="T19" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T19" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>J</v>
+        <v>Q</v>
       </c>
       <c r="U19" s="7"/>
       <c r="V19" s="5"/>
@@ -24681,7 +24684,7 @@
       <c r="AB19" s="5"/>
     </row>
     <row r="20" spans="1:28" ht="15.75">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="15" t="s">
         <v>619</v>
       </c>
       <c r="G20" t="s">
@@ -24696,7 +24699,7 @@
       </c>
       <c r="T20" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T20" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>J</v>
+        <v>I</v>
       </c>
       <c r="U20" s="7"/>
       <c r="V20" s="5"/>
@@ -24706,7 +24709,7 @@
       <c r="AB20" s="5"/>
     </row>
     <row r="21" spans="1:28" ht="15.75">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="15" t="s">
         <v>620</v>
       </c>
       <c r="G21" t="s">
@@ -24721,7 +24724,7 @@
       </c>
       <c r="T21" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T21" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>E</v>
+        <v>X</v>
       </c>
       <c r="U21" s="7"/>
       <c r="V21" s="5"/>
@@ -24731,7 +24734,7 @@
       <c r="AB21" s="5"/>
     </row>
     <row r="22" spans="1:28" ht="15.75">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="15" t="s">
         <v>621</v>
       </c>
       <c r="G22" t="s">
@@ -24746,7 +24749,7 @@
       </c>
       <c r="T22" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T22" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>a</v>
+        <v>b</v>
       </c>
       <c r="U22" s="7"/>
       <c r="V22" s="5"/>
@@ -24756,7 +24759,7 @@
       <c r="AB22" s="5"/>
     </row>
     <row r="23" spans="1:28" ht="15.75">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="15" t="s">
         <v>622</v>
       </c>
       <c r="G23" t="s">
@@ -24771,7 +24774,7 @@
       </c>
       <c r="T23" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T23" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>t</v>
+        <v>L</v>
       </c>
       <c r="U23" s="7"/>
       <c r="V23" s="5"/>
@@ -24781,7 +24784,7 @@
       <c r="AB23" s="5"/>
     </row>
     <row r="24" spans="1:28" ht="15.75">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="15" t="s">
         <v>623</v>
       </c>
       <c r="G24" t="s">
@@ -24796,7 +24799,7 @@
       </c>
       <c r="T24" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T24" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>a</v>
+        <v>u</v>
       </c>
       <c r="U24" s="7"/>
       <c r="V24" s="5"/>
@@ -24806,7 +24809,7 @@
       <c r="AB24" s="5"/>
     </row>
     <row r="25" spans="1:28" ht="15.75">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="15" t="s">
         <v>410</v>
       </c>
       <c r="G25" t="s">
@@ -24821,7 +24824,7 @@
       </c>
       <c r="T25" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T25" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>C</v>
+        <v>J</v>
       </c>
       <c r="U25" s="7"/>
       <c r="V25" s="5"/>
@@ -24831,7 +24834,7 @@
       <c r="AB25" s="5"/>
     </row>
     <row r="26" spans="1:28" ht="15.75">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="15" t="s">
         <v>624</v>
       </c>
       <c r="G26" t="s">
@@ -24846,7 +24849,7 @@
       </c>
       <c r="T26" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T26" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>P</v>
+        <v>H</v>
       </c>
       <c r="U26" s="7"/>
       <c r="V26" s="5"/>
@@ -24856,7 +24859,7 @@
       <c r="AB26" s="5"/>
     </row>
     <row r="27" spans="1:28" ht="15.75">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="15" t="s">
         <v>625</v>
       </c>
       <c r="G27" t="s">
@@ -24871,7 +24874,7 @@
       </c>
       <c r="T27" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T27" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>T</v>
+        <v>o</v>
       </c>
       <c r="U27" s="7"/>
       <c r="V27" s="5"/>
@@ -24881,7 +24884,7 @@
       <c r="AB27" s="5"/>
     </row>
     <row r="28" spans="1:28" ht="15.75">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="15" t="s">
         <v>626</v>
       </c>
       <c r="G28" t="s">
@@ -24903,7 +24906,7 @@
       <c r="AB28" s="5"/>
     </row>
     <row r="29" spans="1:28" ht="15.75">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="15" t="s">
         <v>627</v>
       </c>
       <c r="G29" t="s">
@@ -24925,7 +24928,7 @@
       <c r="AB29" s="5"/>
     </row>
     <row r="30" spans="1:28" ht="15.75">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="15" t="s">
         <v>628</v>
       </c>
       <c r="G30" t="s">
@@ -24940,7 +24943,7 @@
       </c>
       <c r="T30" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T30" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>%</v>
+        <v>d</v>
       </c>
       <c r="U30" s="7"/>
       <c r="V30" s="5"/>
@@ -24950,7 +24953,7 @@
       <c r="AB30" s="5"/>
     </row>
     <row r="31" spans="1:28" ht="15.75">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="15" t="s">
         <v>629</v>
       </c>
       <c r="G31" t="s">
@@ -24965,7 +24968,7 @@
       </c>
       <c r="T31" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T31" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>Z</v>
+        <v>X</v>
       </c>
       <c r="U31" s="7"/>
       <c r="V31" s="5"/>
@@ -24975,7 +24978,7 @@
       <c r="AB31" s="5"/>
     </row>
     <row r="32" spans="1:28" ht="15.75">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="15" t="s">
         <v>630</v>
       </c>
       <c r="G32" t="s">
@@ -24990,7 +24993,7 @@
       </c>
       <c r="T32" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T32" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>b</v>
+        <v>^</v>
       </c>
       <c r="U32" s="7"/>
       <c r="V32" s="5"/>
@@ -25000,7 +25003,7 @@
       <c r="AB32" s="5"/>
     </row>
     <row r="33" spans="1:28" ht="15.75">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="15" t="s">
         <v>631</v>
       </c>
       <c r="G33" t="s">
@@ -25013,9 +25016,9 @@
       <c r="S33" s="5" t="s">
         <v>566</v>
       </c>
-      <c r="T33" s="5" t="str" cm="1">
+      <c r="T33" s="5" cm="1">
         <f t="array" aca="1" ref="T33" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>d</v>
+        <v>1</v>
       </c>
       <c r="U33" s="7"/>
       <c r="V33" s="5"/>
@@ -25025,7 +25028,7 @@
       <c r="AB33" s="5"/>
     </row>
     <row r="34" spans="1:28" ht="15.75">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="15" t="s">
         <v>632</v>
       </c>
       <c r="G34" t="s">
@@ -25050,7 +25053,7 @@
       <c r="AB34" s="5"/>
     </row>
     <row r="35" spans="1:28" ht="15.75">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="15" t="s">
         <v>633</v>
       </c>
       <c r="G35" t="s">
@@ -25065,7 +25068,7 @@
       </c>
       <c r="T35" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T35" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>H</v>
+        <v>p</v>
       </c>
       <c r="U35" s="7"/>
       <c r="V35" s="5"/>
@@ -25075,7 +25078,7 @@
       <c r="AB35" s="5"/>
     </row>
     <row r="36" spans="1:28" ht="15.75">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="15" t="s">
         <v>634</v>
       </c>
       <c r="G36" t="s">
@@ -25090,7 +25093,7 @@
       </c>
       <c r="T36" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T36" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>%</v>
+        <v>v</v>
       </c>
       <c r="U36" s="7"/>
       <c r="V36" s="5"/>
@@ -25100,7 +25103,7 @@
       <c r="AB36" s="5"/>
     </row>
     <row r="37" spans="1:28" ht="15.75">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="15" t="s">
         <v>635</v>
       </c>
       <c r="G37" t="s">
@@ -25115,11 +25118,11 @@
       </c>
       <c r="T37" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T37" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>I</v>
+        <v>c</v>
       </c>
       <c r="U37" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T44)</f>
-        <v>%Zbd7H%I3NnOd1t</v>
+        <v>dX^17pvcimjzU$8</v>
       </c>
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
@@ -25128,7 +25131,7 @@
       <c r="AB37" s="5"/>
     </row>
     <row r="38" spans="1:28" ht="15.75">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="15" t="s">
         <v>636</v>
       </c>
       <c r="G38" t="s">
@@ -25141,13 +25144,13 @@
       <c r="S38" s="5" t="s">
         <v>575</v>
       </c>
-      <c r="T38" s="5" cm="1">
+      <c r="T38" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T38" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>3</v>
+        <v>i</v>
       </c>
       <c r="U38" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T45)</f>
-        <v>%Zbd7H%I3NnOd1tg</v>
+        <v>dX^17pvcimjzU$8*</v>
       </c>
       <c r="V38" s="5"/>
       <c r="W38" s="5"/>
@@ -25156,7 +25159,7 @@
       <c r="AB38" s="5"/>
     </row>
     <row r="39" spans="1:28" ht="15.75">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="15" t="s">
         <v>637</v>
       </c>
       <c r="M39" t="s">
@@ -25168,11 +25171,11 @@
       </c>
       <c r="T39" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T39" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>N</v>
+        <v>m</v>
       </c>
       <c r="U39" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T46)</f>
-        <v>%Zbd7H%I3NnOd1tgp</v>
+        <v>dX^17pvcimjzU$8*S</v>
       </c>
       <c r="V39" s="5"/>
       <c r="W39" s="5"/>
@@ -25181,7 +25184,7 @@
       <c r="AB39" s="5"/>
     </row>
     <row r="40" spans="1:28" ht="15.75">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="15" t="s">
         <v>638</v>
       </c>
       <c r="M40" t="s">
@@ -25193,11 +25196,11 @@
       </c>
       <c r="T40" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T40" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>n</v>
+        <v>j</v>
       </c>
       <c r="U40" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T47)</f>
-        <v>%Zbd7H%I3NnOd1tgp@</v>
+        <v>dX^17pvcimjzU$8*S2</v>
       </c>
       <c r="V40" s="5"/>
       <c r="W40" s="5"/>
@@ -25206,7 +25209,7 @@
       <c r="AB40" s="5"/>
     </row>
     <row r="41" spans="1:28" ht="15.75">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="15" t="s">
         <v>639</v>
       </c>
       <c r="M41" t="s">
@@ -25218,11 +25221,11 @@
       </c>
       <c r="T41" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T41" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>O</v>
+        <v>z</v>
       </c>
       <c r="U41" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T48)</f>
-        <v>%Zbd7H%I3NnOd1tgp@g</v>
+        <v>dX^17pvcimjzU$8*S2H</v>
       </c>
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
@@ -25231,7 +25234,7 @@
       <c r="AB41" s="5"/>
     </row>
     <row r="42" spans="1:28" ht="15.75">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="15" t="s">
         <v>640</v>
       </c>
       <c r="M42" t="s">
@@ -25243,11 +25246,11 @@
       </c>
       <c r="T42" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T42" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>d</v>
+        <v>U</v>
       </c>
       <c r="U42" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T49)</f>
-        <v>%Zbd7H%I3NnOd1tgp@go</v>
+        <v>dX^17pvcimjzU$8*S2Hw</v>
       </c>
       <c r="V42" s="5"/>
       <c r="W42" s="5"/>
@@ -25256,7 +25259,7 @@
       <c r="AB42" s="5"/>
     </row>
     <row r="43" spans="1:28" ht="15.75">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="15" t="s">
         <v>641</v>
       </c>
       <c r="M43" t="s">
@@ -25266,13 +25269,13 @@
       <c r="S43" s="5" t="s">
         <v>577</v>
       </c>
-      <c r="T43" s="5" cm="1">
+      <c r="T43" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T43" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>1</v>
+        <v>$</v>
       </c>
       <c r="U43" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T50)</f>
-        <v>%Zbd7H%I3NnOd1tgp@goj</v>
+        <v>dX^17pvcimjzU$8*S2Hw6</v>
       </c>
       <c r="V43" s="5"/>
       <c r="W43" s="5"/>
@@ -25281,7 +25284,7 @@
       <c r="AB43" s="5"/>
     </row>
     <row r="44" spans="1:28" ht="15.75">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="15" t="s">
         <v>642</v>
       </c>
       <c r="M44" t="s">
@@ -25291,13 +25294,13 @@
       <c r="S44" s="5" t="s">
         <v>578</v>
       </c>
-      <c r="T44" s="5" t="str" cm="1">
+      <c r="T44" s="5" cm="1">
         <f t="array" aca="1" ref="T44" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>t</v>
+        <v>8</v>
       </c>
       <c r="U44" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T51)</f>
-        <v>%Zbd7H%I3NnOd1tgp@gojG</v>
+        <v>dX^17pvcimjzU$8*S2Hw6V</v>
       </c>
       <c r="V44" s="5"/>
       <c r="W44" s="5"/>
@@ -25306,7 +25309,7 @@
       <c r="AB44" s="5"/>
     </row>
     <row r="45" spans="1:28" ht="15.75">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="15" t="s">
         <v>643</v>
       </c>
       <c r="M45" t="s">
@@ -25318,11 +25321,11 @@
       </c>
       <c r="T45" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T45" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>g</v>
+        <v>*</v>
       </c>
       <c r="U45" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T52)</f>
-        <v>%Zbd7H%I3NnOd1tgp@gojGt</v>
+        <v>dX^17pvcimjzU$8*S2Hw6Vw</v>
       </c>
       <c r="V45" s="5"/>
       <c r="W45" s="5"/>
@@ -25331,7 +25334,7 @@
       <c r="AB45" s="5"/>
     </row>
     <row r="46" spans="1:28" ht="15.75">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="15" t="s">
         <v>644</v>
       </c>
       <c r="M46" t="s">
@@ -25343,11 +25346,11 @@
       </c>
       <c r="T46" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T46" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>p</v>
+        <v>S</v>
       </c>
       <c r="U46" s="7" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T53)</f>
-        <v>%Zbd7H%I3NnOd1tgp@gojGt3</v>
+        <v>dX^17pvcimjzU$8*S2Hw6Vwh</v>
       </c>
       <c r="V46" s="5"/>
       <c r="W46" s="5"/>
@@ -25356,7 +25359,7 @@
       <c r="AB46" s="5"/>
     </row>
     <row r="47" spans="1:28" ht="15.75">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="15" t="s">
         <v>645</v>
       </c>
       <c r="M47" t="s">
@@ -25366,9 +25369,9 @@
       <c r="S47" s="5" t="s">
         <v>581</v>
       </c>
-      <c r="T47" s="5" t="str" cm="1">
+      <c r="T47" s="5" cm="1">
         <f t="array" aca="1" ref="T47" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>@</v>
+        <v>2</v>
       </c>
       <c r="U47" s="7"/>
       <c r="V47" s="5"/>
@@ -25378,7 +25381,7 @@
       <c r="AB47" s="5"/>
     </row>
     <row r="48" spans="1:28" ht="15.75">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="15" t="s">
         <v>646</v>
       </c>
       <c r="M48" t="s">
@@ -25390,7 +25393,7 @@
       </c>
       <c r="T48" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T48" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>g</v>
+        <v>H</v>
       </c>
       <c r="U48" s="7"/>
       <c r="V48" s="5"/>
@@ -25400,7 +25403,7 @@
       <c r="AB48" s="5"/>
     </row>
     <row r="49" spans="1:28" ht="15.75">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="15" t="s">
         <v>647</v>
       </c>
       <c r="M49" t="s">
@@ -25412,7 +25415,7 @@
       </c>
       <c r="T49" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T49" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>o</v>
+        <v>w</v>
       </c>
       <c r="U49" s="7"/>
       <c r="V49" s="5"/>
@@ -25422,7 +25425,7 @@
       <c r="AB49" s="5"/>
     </row>
     <row r="50" spans="1:28" ht="15.75">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="15" t="s">
         <v>648</v>
       </c>
       <c r="M50" t="s">
@@ -25432,9 +25435,9 @@
       <c r="S50" s="5" t="s">
         <v>584</v>
       </c>
-      <c r="T50" s="5" t="str" cm="1">
+      <c r="T50" s="5" cm="1">
         <f t="array" aca="1" ref="T50" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>j</v>
+        <v>6</v>
       </c>
       <c r="U50" s="7"/>
       <c r="V50" s="5"/>
@@ -25444,7 +25447,7 @@
       <c r="AB50" s="5"/>
     </row>
     <row r="51" spans="1:28" ht="15.75">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="15" t="s">
         <v>649</v>
       </c>
       <c r="M51" t="s">
@@ -25456,7 +25459,7 @@
       </c>
       <c r="T51" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T51" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>G</v>
+        <v>V</v>
       </c>
       <c r="U51" s="7"/>
       <c r="V51" s="5"/>
@@ -25466,7 +25469,7 @@
       <c r="AB51" s="5"/>
     </row>
     <row r="52" spans="1:28" ht="15.75">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="15" t="s">
         <v>650</v>
       </c>
       <c r="M52" t="s">
@@ -25478,7 +25481,7 @@
       </c>
       <c r="T52" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T52" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>t</v>
+        <v>w</v>
       </c>
       <c r="U52" s="7"/>
       <c r="V52" s="5"/>
@@ -25488,7 +25491,7 @@
       <c r="AB52" s="5"/>
     </row>
     <row r="53" spans="1:28" ht="15.75">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="15" t="s">
         <v>651</v>
       </c>
       <c r="M53" t="s">
@@ -25498,9 +25501,9 @@
       <c r="S53" s="5" t="s">
         <v>587</v>
       </c>
-      <c r="T53" s="5" cm="1">
+      <c r="T53" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="T53" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>3</v>
+        <v>h</v>
       </c>
       <c r="V53" s="5"/>
       <c r="W53" s="5"/>
@@ -25718,8 +25721,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25741,11 +25745,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>430</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -26332,11 +26336,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>434</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Updated users and made a duplicate patient
</commit_message>
<xml_diff>
--- a/Database Data.xlsx
+++ b/Database Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\futur\Documents\GitHub\CIS424_wi21_Med_Cart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Capstone\Capstone_wi21_project\CIS424_wi21_Med_Cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EE09E5-AE3D-4D3B-8F03-C8AF53000DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C018FD36-584F-492C-B9A0-5F6ECEFCCAEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3326" uniqueCount="1509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3500" uniqueCount="1610">
   <si>
     <t>User</t>
   </si>
@@ -4594,6 +4594,309 @@
   </si>
   <si>
     <t>PatientPhysician</t>
+  </si>
+  <si>
+    <t>xSHRcaSTVZkjoWA58</t>
+  </si>
+  <si>
+    <t>Student1</t>
+  </si>
+  <si>
+    <t>Student2</t>
+  </si>
+  <si>
+    <t>Student3</t>
+  </si>
+  <si>
+    <t>Student4</t>
+  </si>
+  <si>
+    <t>Student5</t>
+  </si>
+  <si>
+    <t>Student6</t>
+  </si>
+  <si>
+    <t>Student7</t>
+  </si>
+  <si>
+    <t>Student8</t>
+  </si>
+  <si>
+    <t>Student9</t>
+  </si>
+  <si>
+    <t>Student10</t>
+  </si>
+  <si>
+    <t>Student11</t>
+  </si>
+  <si>
+    <t>Student12</t>
+  </si>
+  <si>
+    <t>Student13</t>
+  </si>
+  <si>
+    <t>Student14</t>
+  </si>
+  <si>
+    <t>Student15</t>
+  </si>
+  <si>
+    <t>Student16</t>
+  </si>
+  <si>
+    <t>Student17</t>
+  </si>
+  <si>
+    <t>Student18</t>
+  </si>
+  <si>
+    <t>Student19</t>
+  </si>
+  <si>
+    <t>Student20</t>
+  </si>
+  <si>
+    <t>Student21</t>
+  </si>
+  <si>
+    <t>Student22</t>
+  </si>
+  <si>
+    <t>Student23</t>
+  </si>
+  <si>
+    <t>Student24</t>
+  </si>
+  <si>
+    <t>Student25</t>
+  </si>
+  <si>
+    <t>Student26</t>
+  </si>
+  <si>
+    <t>Student27</t>
+  </si>
+  <si>
+    <t>Student28</t>
+  </si>
+  <si>
+    <t>Student29</t>
+  </si>
+  <si>
+    <t>Student30</t>
+  </si>
+  <si>
+    <t>Instructor1</t>
+  </si>
+  <si>
+    <t>Instructor2</t>
+  </si>
+  <si>
+    <t>Instructor3</t>
+  </si>
+  <si>
+    <t>Student01Password!</t>
+  </si>
+  <si>
+    <t>Student02Password!</t>
+  </si>
+  <si>
+    <t>Student03Password!</t>
+  </si>
+  <si>
+    <t>Student04Password!</t>
+  </si>
+  <si>
+    <t>Student05Password!</t>
+  </si>
+  <si>
+    <t>Student06Password!</t>
+  </si>
+  <si>
+    <t>Student07Password!</t>
+  </si>
+  <si>
+    <t>Student08Password!</t>
+  </si>
+  <si>
+    <t>Student09Password!</t>
+  </si>
+  <si>
+    <t>Student10Password!</t>
+  </si>
+  <si>
+    <t>Student11Password!</t>
+  </si>
+  <si>
+    <t>Student12Password!</t>
+  </si>
+  <si>
+    <t>Student13Password!</t>
+  </si>
+  <si>
+    <t>Student14Password!</t>
+  </si>
+  <si>
+    <t>Student15Password!</t>
+  </si>
+  <si>
+    <t>Student16Password!</t>
+  </si>
+  <si>
+    <t>Student17Password!</t>
+  </si>
+  <si>
+    <t>Student18Password!</t>
+  </si>
+  <si>
+    <t>Student19Password!</t>
+  </si>
+  <si>
+    <t>Student20Password!</t>
+  </si>
+  <si>
+    <t>Student21Password!</t>
+  </si>
+  <si>
+    <t>Student22Password!</t>
+  </si>
+  <si>
+    <t>Student23Password!</t>
+  </si>
+  <si>
+    <t>Student24Password!</t>
+  </si>
+  <si>
+    <t>Student25Password!</t>
+  </si>
+  <si>
+    <t>Student26Password!</t>
+  </si>
+  <si>
+    <t>Student27Password!</t>
+  </si>
+  <si>
+    <t>Student28Password!</t>
+  </si>
+  <si>
+    <t>Student29Password!</t>
+  </si>
+  <si>
+    <t>Student30Password!</t>
+  </si>
+  <si>
+    <t>Instructor1Password!</t>
+  </si>
+  <si>
+    <t>Instructor2Password!</t>
+  </si>
+  <si>
+    <t>SVSU</t>
+  </si>
+  <si>
+    <t>Instructor3Password!</t>
+  </si>
+  <si>
+    <t>Student01B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student02B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student03B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student04B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student05B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student06B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student07B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student08B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student09B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student10B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student11B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student12B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student13B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student14B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student15B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student16B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student17B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student18B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student19B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student20B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student21B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student22B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student23B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student24B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student25B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student26B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student27B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student28B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student29B@rc0D#</t>
+  </si>
+  <si>
+    <t>Student30B@rc0D#</t>
+  </si>
+  <si>
+    <t>Instructor01B@rc0D#</t>
+  </si>
+  <si>
+    <t>Instructor02B@rc0D#</t>
+  </si>
+  <si>
+    <t>Instructor03B@rc0D#</t>
   </si>
 </sst>
 </file>
@@ -4746,7 +5049,77 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6F599AD3-6840-46F2-88F2-0E9C6FEC8D7E}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{099EC489-0DCF-455E-884E-0F2FAB91D948}"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="55">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5505,15 +5878,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG161"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.140625" style="7" bestFit="1" customWidth="1"/>
@@ -12302,12 +12675,33 @@
       <c r="BG102" s="4"/>
     </row>
     <row r="103" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A103" s="4"/>
-      <c r="B103" s="5"/>
-      <c r="F103" s="8"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="4"/>
+      <c r="A103" s="4">
+        <v>110</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>1543</v>
+      </c>
+      <c r="D103" t="s">
+        <v>1510</v>
+      </c>
+      <c r="E103" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>1577</v>
+      </c>
+      <c r="G103" s="4">
+        <v>0</v>
+      </c>
+      <c r="H103" s="4">
+        <v>0</v>
+      </c>
+      <c r="I103" s="4">
+        <v>1</v>
+      </c>
       <c r="J103" s="5"/>
       <c r="K103" s="5"/>
       <c r="L103" s="4"/>
@@ -12339,15 +12733,33 @@
       <c r="BG103" s="4"/>
     </row>
     <row r="104" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="4"/>
-      <c r="D104" s="4"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="8"/>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
+      <c r="A104" s="4">
+        <v>111</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>1511</v>
+      </c>
+      <c r="E104" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>1578</v>
+      </c>
+      <c r="G104" s="4">
+        <v>0</v>
+      </c>
+      <c r="H104" s="4">
+        <v>0</v>
+      </c>
+      <c r="I104" s="4">
+        <v>1</v>
+      </c>
       <c r="J104" s="5"/>
       <c r="K104" s="5"/>
       <c r="L104" s="4"/>
@@ -12379,10 +12791,33 @@
       <c r="BG104" s="4"/>
     </row>
     <row r="105" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B105" s="5"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4"/>
-      <c r="I105" s="4"/>
+      <c r="A105" s="4">
+        <v>112</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1512</v>
+      </c>
+      <c r="E105" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>1579</v>
+      </c>
+      <c r="G105" s="4">
+        <v>0</v>
+      </c>
+      <c r="H105" s="4">
+        <v>0</v>
+      </c>
+      <c r="I105" s="4">
+        <v>1</v>
+      </c>
       <c r="J105" s="5"/>
       <c r="K105" s="5"/>
       <c r="L105" s="4"/>
@@ -12414,11 +12849,33 @@
       <c r="BG105" s="4"/>
     </row>
     <row r="106" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B106" s="5"/>
-      <c r="D106" s="1"/>
-      <c r="G106" s="4"/>
-      <c r="H106" s="4"/>
-      <c r="I106" s="4"/>
+      <c r="A106" s="4">
+        <v>113</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>1546</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>1513</v>
+      </c>
+      <c r="E106" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>1580</v>
+      </c>
+      <c r="G106" s="4">
+        <v>0</v>
+      </c>
+      <c r="H106" s="4">
+        <v>0</v>
+      </c>
+      <c r="I106" s="4">
+        <v>1</v>
+      </c>
       <c r="J106" s="5"/>
       <c r="K106" s="5"/>
       <c r="L106" s="4"/>
@@ -12450,11 +12907,33 @@
       <c r="BG106" s="4"/>
     </row>
     <row r="107" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B107" s="5"/>
-      <c r="D107" s="1"/>
-      <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
-      <c r="I107" s="4"/>
+      <c r="A107" s="4">
+        <v>114</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>1547</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>1514</v>
+      </c>
+      <c r="E107" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G107" s="4">
+        <v>0</v>
+      </c>
+      <c r="H107" s="4">
+        <v>0</v>
+      </c>
+      <c r="I107" s="4">
+        <v>1</v>
+      </c>
       <c r="J107" s="5"/>
       <c r="K107" s="5"/>
       <c r="L107" s="4"/>
@@ -12486,10 +12965,33 @@
       <c r="BG107" s="4"/>
     </row>
     <row r="108" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D108" s="1"/>
-      <c r="G108" s="4"/>
-      <c r="H108" s="4"/>
-      <c r="I108" s="4"/>
+      <c r="A108" s="4">
+        <v>115</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>1515</v>
+      </c>
+      <c r="E108" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>1582</v>
+      </c>
+      <c r="G108" s="4">
+        <v>0</v>
+      </c>
+      <c r="H108" s="4">
+        <v>0</v>
+      </c>
+      <c r="I108" s="4">
+        <v>1</v>
+      </c>
       <c r="J108" s="5"/>
       <c r="K108" s="5"/>
       <c r="L108" s="4"/>
@@ -12521,10 +13023,33 @@
       <c r="BG108" s="4"/>
     </row>
     <row r="109" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D109" s="1"/>
-      <c r="G109" s="4"/>
-      <c r="H109" s="4"/>
-      <c r="I109" s="4"/>
+      <c r="A109" s="4">
+        <v>116</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>1549</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>1516</v>
+      </c>
+      <c r="E109" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>1583</v>
+      </c>
+      <c r="G109" s="4">
+        <v>0</v>
+      </c>
+      <c r="H109" s="4">
+        <v>0</v>
+      </c>
+      <c r="I109" s="4">
+        <v>1</v>
+      </c>
       <c r="J109" s="5"/>
       <c r="K109" s="5"/>
       <c r="L109" s="4"/>
@@ -12556,10 +13081,33 @@
       <c r="BG109" s="4"/>
     </row>
     <row r="110" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D110" s="1"/>
-      <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
-      <c r="I110" s="4"/>
+      <c r="A110" s="4">
+        <v>117</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>1517</v>
+      </c>
+      <c r="E110" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>1584</v>
+      </c>
+      <c r="G110" s="4">
+        <v>0</v>
+      </c>
+      <c r="H110" s="4">
+        <v>0</v>
+      </c>
+      <c r="I110" s="4">
+        <v>1</v>
+      </c>
       <c r="J110" s="5"/>
       <c r="K110" s="5"/>
       <c r="L110" s="4"/>
@@ -12591,10 +13139,33 @@
       <c r="BG110" s="4"/>
     </row>
     <row r="111" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D111" s="1"/>
-      <c r="G111" s="4"/>
-      <c r="H111" s="4"/>
-      <c r="I111" s="4"/>
+      <c r="A111" s="4">
+        <v>119</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>1551</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E111" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>1585</v>
+      </c>
+      <c r="G111" s="4">
+        <v>0</v>
+      </c>
+      <c r="H111" s="4">
+        <v>0</v>
+      </c>
+      <c r="I111" s="4">
+        <v>1</v>
+      </c>
       <c r="J111" s="5"/>
       <c r="K111" s="5"/>
       <c r="L111" s="4"/>
@@ -12626,10 +13197,33 @@
       <c r="BG111" s="4"/>
     </row>
     <row r="112" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D112" s="1"/>
-      <c r="G112" s="4"/>
-      <c r="H112" s="4"/>
-      <c r="I112" s="4"/>
+      <c r="A112" s="4">
+        <v>120</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>1552</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>1519</v>
+      </c>
+      <c r="E112" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>1586</v>
+      </c>
+      <c r="G112" s="4">
+        <v>0</v>
+      </c>
+      <c r="H112" s="4">
+        <v>0</v>
+      </c>
+      <c r="I112" s="4">
+        <v>1</v>
+      </c>
       <c r="J112" s="5"/>
       <c r="K112" s="5"/>
       <c r="L112" s="4"/>
@@ -12661,10 +13255,33 @@
       <c r="BG112" s="4"/>
     </row>
     <row r="113" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D113" s="1"/>
-      <c r="G113" s="4"/>
-      <c r="H113" s="4"/>
-      <c r="I113" s="4"/>
+      <c r="A113" s="4">
+        <v>121</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="E113" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>1587</v>
+      </c>
+      <c r="G113" s="4">
+        <v>0</v>
+      </c>
+      <c r="H113" s="4">
+        <v>0</v>
+      </c>
+      <c r="I113" s="4">
+        <v>1</v>
+      </c>
       <c r="J113" s="5"/>
       <c r="K113" s="5"/>
       <c r="L113" s="4"/>
@@ -12696,10 +13313,33 @@
       <c r="BG113" s="4"/>
     </row>
     <row r="114" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D114" s="1"/>
-      <c r="G114" s="4"/>
-      <c r="H114" s="16"/>
-      <c r="I114" s="4"/>
+      <c r="A114" s="4">
+        <v>122</v>
+      </c>
+      <c r="B114" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>1554</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>1521</v>
+      </c>
+      <c r="E114" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>1588</v>
+      </c>
+      <c r="G114" s="4">
+        <v>0</v>
+      </c>
+      <c r="H114" s="4">
+        <v>0</v>
+      </c>
+      <c r="I114" s="4">
+        <v>1</v>
+      </c>
       <c r="J114" s="5"/>
       <c r="K114" s="5"/>
       <c r="L114" s="4"/>
@@ -12731,10 +13371,33 @@
       <c r="BG114" s="4"/>
     </row>
     <row r="115" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D115" s="1"/>
-      <c r="G115" s="4"/>
-      <c r="H115" s="4"/>
-      <c r="I115" s="4"/>
+      <c r="A115" s="4">
+        <v>123</v>
+      </c>
+      <c r="B115" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>1555</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>1522</v>
+      </c>
+      <c r="E115" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G115" s="4">
+        <v>0</v>
+      </c>
+      <c r="H115" s="4">
+        <v>0</v>
+      </c>
+      <c r="I115" s="4">
+        <v>1</v>
+      </c>
       <c r="J115" s="5"/>
       <c r="K115" s="5"/>
       <c r="L115" s="4"/>
@@ -12766,10 +13429,33 @@
       <c r="BG115" s="4"/>
     </row>
     <row r="116" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D116" s="1"/>
-      <c r="G116" s="4"/>
-      <c r="H116" s="4"/>
-      <c r="I116" s="4"/>
+      <c r="A116" s="4">
+        <v>124</v>
+      </c>
+      <c r="B116" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>1556</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>1523</v>
+      </c>
+      <c r="E116" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>1590</v>
+      </c>
+      <c r="G116" s="4">
+        <v>0</v>
+      </c>
+      <c r="H116" s="4">
+        <v>0</v>
+      </c>
+      <c r="I116" s="4">
+        <v>1</v>
+      </c>
       <c r="J116" s="5"/>
       <c r="K116" s="5"/>
       <c r="L116" s="4"/>
@@ -12801,10 +13487,33 @@
       <c r="BG116" s="4"/>
     </row>
     <row r="117" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D117" s="1"/>
-      <c r="G117" s="4"/>
-      <c r="H117" s="4"/>
-      <c r="I117" s="4"/>
+      <c r="A117" s="4">
+        <v>125</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>1557</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>1524</v>
+      </c>
+      <c r="E117" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G117" s="4">
+        <v>0</v>
+      </c>
+      <c r="H117" s="4">
+        <v>0</v>
+      </c>
+      <c r="I117" s="4">
+        <v>1</v>
+      </c>
       <c r="J117" s="5"/>
       <c r="K117" s="5"/>
       <c r="L117" s="4"/>
@@ -12836,10 +13545,33 @@
       <c r="BG117" s="4"/>
     </row>
     <row r="118" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D118" s="1"/>
-      <c r="G118" s="4"/>
-      <c r="H118" s="4"/>
-      <c r="I118" s="4"/>
+      <c r="A118" s="4">
+        <v>126</v>
+      </c>
+      <c r="B118" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="E118" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F118" s="7" t="s">
+        <v>1592</v>
+      </c>
+      <c r="G118" s="4">
+        <v>0</v>
+      </c>
+      <c r="H118" s="4">
+        <v>0</v>
+      </c>
+      <c r="I118" s="4">
+        <v>1</v>
+      </c>
       <c r="J118" s="5"/>
       <c r="K118" s="5"/>
       <c r="L118" s="4"/>
@@ -12848,10 +13580,33 @@
       <c r="Q118" s="5"/>
     </row>
     <row r="119" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D119" s="1"/>
-      <c r="G119" s="4"/>
-      <c r="H119" s="4"/>
-      <c r="I119" s="4"/>
+      <c r="A119" s="4">
+        <v>127</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>1559</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>1526</v>
+      </c>
+      <c r="E119" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F119" s="7" t="s">
+        <v>1593</v>
+      </c>
+      <c r="G119" s="4">
+        <v>0</v>
+      </c>
+      <c r="H119" s="4">
+        <v>0</v>
+      </c>
+      <c r="I119" s="4">
+        <v>1</v>
+      </c>
       <c r="J119" s="5"/>
       <c r="K119" s="5"/>
       <c r="L119" s="4"/>
@@ -12860,15 +13615,33 @@
       <c r="Q119" s="5"/>
     </row>
     <row r="120" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A120" s="4"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4"/>
-      <c r="E120" s="4"/>
-      <c r="F120" s="8"/>
-      <c r="G120" s="4"/>
-      <c r="H120" s="4"/>
-      <c r="I120" s="4"/>
+      <c r="A120" s="4">
+        <v>128</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>1527</v>
+      </c>
+      <c r="E120" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>1594</v>
+      </c>
+      <c r="G120" s="4">
+        <v>0</v>
+      </c>
+      <c r="H120" s="4">
+        <v>0</v>
+      </c>
+      <c r="I120" s="4">
+        <v>1</v>
+      </c>
       <c r="J120" s="5"/>
       <c r="K120" s="5"/>
       <c r="L120" s="4"/>
@@ -12877,15 +13650,33 @@
       <c r="Q120" s="5"/>
     </row>
     <row r="121" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A121" s="4"/>
-      <c r="B121" s="5"/>
-      <c r="C121" s="4"/>
-      <c r="D121" s="4"/>
-      <c r="E121" s="4"/>
-      <c r="F121" s="8"/>
-      <c r="G121" s="4"/>
-      <c r="H121" s="4"/>
-      <c r="I121" s="4"/>
+      <c r="A121" s="4">
+        <v>129</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>1528</v>
+      </c>
+      <c r="E121" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F121" s="7" t="s">
+        <v>1595</v>
+      </c>
+      <c r="G121" s="4">
+        <v>0</v>
+      </c>
+      <c r="H121" s="4">
+        <v>0</v>
+      </c>
+      <c r="I121" s="4">
+        <v>1</v>
+      </c>
       <c r="J121" s="5"/>
       <c r="K121" s="5"/>
       <c r="L121" s="4"/>
@@ -12894,15 +13685,33 @@
       <c r="Q121" s="5"/>
     </row>
     <row r="122" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A122" s="4"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="4"/>
-      <c r="E122" s="4"/>
-      <c r="F122" s="8"/>
-      <c r="G122" s="4"/>
-      <c r="H122" s="4"/>
-      <c r="I122" s="4"/>
+      <c r="A122" s="4">
+        <v>130</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>1529</v>
+      </c>
+      <c r="E122" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F122" s="7" t="s">
+        <v>1596</v>
+      </c>
+      <c r="G122" s="4">
+        <v>0</v>
+      </c>
+      <c r="H122" s="4">
+        <v>0</v>
+      </c>
+      <c r="I122" s="4">
+        <v>1</v>
+      </c>
       <c r="J122" s="5"/>
       <c r="K122" s="5"/>
       <c r="L122" s="4"/>
@@ -12911,15 +13720,33 @@
       <c r="Q122" s="5"/>
     </row>
     <row r="123" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A123" s="4"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="4"/>
-      <c r="D123" s="4"/>
-      <c r="E123" s="4"/>
-      <c r="F123" s="8"/>
-      <c r="G123" s="4"/>
-      <c r="H123" s="4"/>
-      <c r="I123" s="4"/>
+      <c r="A123" s="4">
+        <v>131</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>1563</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>1530</v>
+      </c>
+      <c r="E123" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>1597</v>
+      </c>
+      <c r="G123" s="4">
+        <v>0</v>
+      </c>
+      <c r="H123" s="4">
+        <v>0</v>
+      </c>
+      <c r="I123" s="4">
+        <v>1</v>
+      </c>
       <c r="J123" s="5"/>
       <c r="K123" s="5"/>
       <c r="L123" s="4"/>
@@ -12928,15 +13755,33 @@
       <c r="Q123" s="5"/>
     </row>
     <row r="124" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A124" s="4"/>
-      <c r="B124" s="5"/>
-      <c r="C124" s="4"/>
-      <c r="D124" s="4"/>
-      <c r="E124" s="4"/>
-      <c r="F124" s="8"/>
-      <c r="G124" s="4"/>
-      <c r="H124" s="4"/>
-      <c r="I124" s="4"/>
+      <c r="A124" s="4">
+        <v>132</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="E124" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>1598</v>
+      </c>
+      <c r="G124" s="4">
+        <v>0</v>
+      </c>
+      <c r="H124" s="4">
+        <v>0</v>
+      </c>
+      <c r="I124" s="4">
+        <v>1</v>
+      </c>
       <c r="J124" s="5"/>
       <c r="K124" s="5"/>
       <c r="L124" s="4"/>
@@ -12945,15 +13790,33 @@
       <c r="Q124" s="5"/>
     </row>
     <row r="125" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A125" s="4"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="4"/>
-      <c r="D125" s="4"/>
-      <c r="E125" s="4"/>
-      <c r="F125" s="8"/>
-      <c r="G125" s="4"/>
-      <c r="H125" s="4"/>
-      <c r="I125" s="4"/>
+      <c r="A125" s="4">
+        <v>133</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>1565</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>1532</v>
+      </c>
+      <c r="E125" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>1599</v>
+      </c>
+      <c r="G125" s="4">
+        <v>0</v>
+      </c>
+      <c r="H125" s="4">
+        <v>0</v>
+      </c>
+      <c r="I125" s="4">
+        <v>1</v>
+      </c>
       <c r="J125" s="5"/>
       <c r="K125" s="5"/>
       <c r="L125" s="4"/>
@@ -12962,15 +13825,33 @@
       <c r="Q125" s="5"/>
     </row>
     <row r="126" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A126" s="4"/>
-      <c r="B126" s="5"/>
-      <c r="C126" s="4"/>
-      <c r="D126" s="4"/>
-      <c r="E126" s="4"/>
-      <c r="F126" s="8"/>
-      <c r="G126" s="4"/>
-      <c r="H126" s="4"/>
-      <c r="I126" s="4"/>
+      <c r="A126" s="4">
+        <v>134</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>1566</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>1533</v>
+      </c>
+      <c r="E126" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F126" s="7" t="s">
+        <v>1600</v>
+      </c>
+      <c r="G126" s="4">
+        <v>0</v>
+      </c>
+      <c r="H126" s="4">
+        <v>0</v>
+      </c>
+      <c r="I126" s="4">
+        <v>1</v>
+      </c>
       <c r="J126" s="5"/>
       <c r="K126" s="5"/>
       <c r="L126" s="4"/>
@@ -12979,15 +13860,33 @@
       <c r="Q126" s="5"/>
     </row>
     <row r="127" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A127" s="4"/>
-      <c r="B127" s="5"/>
-      <c r="C127" s="4"/>
-      <c r="D127" s="4"/>
-      <c r="E127" s="4"/>
-      <c r="F127" s="8"/>
-      <c r="G127" s="4"/>
-      <c r="H127" s="4"/>
-      <c r="I127" s="4"/>
+      <c r="A127" s="4">
+        <v>135</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>1567</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E127" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F127" s="7" t="s">
+        <v>1601</v>
+      </c>
+      <c r="G127" s="4">
+        <v>0</v>
+      </c>
+      <c r="H127" s="4">
+        <v>0</v>
+      </c>
+      <c r="I127" s="4">
+        <v>1</v>
+      </c>
       <c r="J127" s="5"/>
       <c r="K127" s="5"/>
       <c r="L127" s="4"/>
@@ -12996,15 +13895,33 @@
       <c r="Q127" s="5"/>
     </row>
     <row r="128" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A128" s="4"/>
-      <c r="B128" s="5"/>
-      <c r="C128" s="4"/>
-      <c r="D128" s="4"/>
-      <c r="E128" s="4"/>
-      <c r="F128" s="8"/>
-      <c r="G128" s="4"/>
-      <c r="H128" s="4"/>
-      <c r="I128" s="4"/>
+      <c r="A128" s="4">
+        <v>136</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E128" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F128" s="7" t="s">
+        <v>1602</v>
+      </c>
+      <c r="G128" s="4">
+        <v>0</v>
+      </c>
+      <c r="H128" s="4">
+        <v>0</v>
+      </c>
+      <c r="I128" s="4">
+        <v>1</v>
+      </c>
       <c r="J128" s="5"/>
       <c r="K128" s="5"/>
       <c r="L128" s="4"/>
@@ -13013,15 +13930,33 @@
       <c r="Q128" s="5"/>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A129" s="4"/>
-      <c r="B129" s="5"/>
-      <c r="C129" s="4"/>
-      <c r="D129" s="4"/>
-      <c r="E129" s="4"/>
-      <c r="F129" s="8"/>
-      <c r="G129" s="4"/>
-      <c r="H129" s="4"/>
-      <c r="I129" s="4"/>
+      <c r="A129" s="4">
+        <v>137</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C129" s="8" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>1536</v>
+      </c>
+      <c r="E129" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F129" s="7" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G129" s="4">
+        <v>0</v>
+      </c>
+      <c r="H129" s="4">
+        <v>0</v>
+      </c>
+      <c r="I129" s="4">
+        <v>1</v>
+      </c>
       <c r="J129" s="5"/>
       <c r="K129" s="5"/>
       <c r="L129" s="4"/>
@@ -13030,15 +13965,33 @@
       <c r="Q129" s="5"/>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A130" s="4"/>
-      <c r="B130" s="5"/>
-      <c r="C130" s="4"/>
-      <c r="D130" s="4"/>
-      <c r="E130" s="4"/>
-      <c r="F130" s="8"/>
-      <c r="G130" s="4"/>
-      <c r="H130" s="4"/>
-      <c r="I130" s="4"/>
+      <c r="A130" s="4">
+        <v>138</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>1570</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>1537</v>
+      </c>
+      <c r="E130" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F130" s="7" t="s">
+        <v>1604</v>
+      </c>
+      <c r="G130" s="4">
+        <v>0</v>
+      </c>
+      <c r="H130" s="4">
+        <v>0</v>
+      </c>
+      <c r="I130" s="4">
+        <v>1</v>
+      </c>
       <c r="J130" s="5"/>
       <c r="K130" s="5"/>
       <c r="L130" s="4"/>
@@ -13047,15 +14000,33 @@
       <c r="Q130" s="5"/>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A131" s="4"/>
-      <c r="B131" s="5"/>
-      <c r="C131" s="4"/>
-      <c r="D131" s="4"/>
-      <c r="E131" s="4"/>
-      <c r="F131" s="8"/>
-      <c r="G131" s="4"/>
-      <c r="H131" s="4"/>
-      <c r="I131" s="4"/>
+      <c r="A131" s="4">
+        <v>139</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C131" s="8" t="s">
+        <v>1571</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>1538</v>
+      </c>
+      <c r="E131" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F131" s="7" t="s">
+        <v>1605</v>
+      </c>
+      <c r="G131" s="4">
+        <v>0</v>
+      </c>
+      <c r="H131" s="4">
+        <v>0</v>
+      </c>
+      <c r="I131" s="4">
+        <v>1</v>
+      </c>
       <c r="J131" s="5"/>
       <c r="K131" s="5"/>
       <c r="L131" s="4"/>
@@ -13064,15 +14035,33 @@
       <c r="Q131" s="5"/>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A132" s="4"/>
-      <c r="B132" s="5"/>
-      <c r="C132" s="4"/>
-      <c r="D132" s="4"/>
-      <c r="E132" s="4"/>
-      <c r="F132" s="8"/>
-      <c r="G132" s="4"/>
-      <c r="H132" s="4"/>
-      <c r="I132" s="4"/>
+      <c r="A132" s="4">
+        <v>140</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>1572</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E132" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F132" s="7" t="s">
+        <v>1606</v>
+      </c>
+      <c r="G132" s="4">
+        <v>0</v>
+      </c>
+      <c r="H132" s="4">
+        <v>0</v>
+      </c>
+      <c r="I132" s="4">
+        <v>1</v>
+      </c>
       <c r="J132" s="5"/>
       <c r="K132" s="5"/>
       <c r="L132" s="4"/>
@@ -13081,15 +14070,33 @@
       <c r="Q132" s="5"/>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A133" s="4"/>
-      <c r="B133" s="5"/>
-      <c r="C133" s="4"/>
-      <c r="D133" s="4"/>
-      <c r="E133" s="4"/>
-      <c r="F133" s="8"/>
-      <c r="G133" s="4"/>
-      <c r="H133" s="4"/>
-      <c r="I133" s="4"/>
+      <c r="A133" s="4">
+        <v>141</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>1573</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>1540</v>
+      </c>
+      <c r="E133" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F133" s="7" t="s">
+        <v>1607</v>
+      </c>
+      <c r="G133" s="4">
+        <v>0</v>
+      </c>
+      <c r="H133" s="4">
+        <v>1</v>
+      </c>
+      <c r="I133" s="4">
+        <v>1</v>
+      </c>
       <c r="J133" s="5"/>
       <c r="K133" s="5"/>
       <c r="L133" s="4"/>
@@ -13098,15 +14105,33 @@
       <c r="Q133" s="5"/>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A134" s="4"/>
-      <c r="B134" s="5"/>
-      <c r="C134" s="4"/>
-      <c r="D134" s="4"/>
-      <c r="E134" s="4"/>
-      <c r="F134" s="8"/>
-      <c r="G134" s="4"/>
-      <c r="H134" s="4"/>
-      <c r="I134" s="4"/>
+      <c r="A134" s="4">
+        <v>142</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>1541</v>
+      </c>
+      <c r="E134" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F134" s="7" t="s">
+        <v>1608</v>
+      </c>
+      <c r="G134" s="4">
+        <v>0</v>
+      </c>
+      <c r="H134" s="4">
+        <v>1</v>
+      </c>
+      <c r="I134" s="4">
+        <v>1</v>
+      </c>
       <c r="J134" s="5"/>
       <c r="K134" s="5"/>
       <c r="L134" s="4"/>
@@ -13115,15 +14140,33 @@
       <c r="Q134" s="5"/>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A135" s="4"/>
-      <c r="B135" s="5"/>
-      <c r="C135" s="4"/>
-      <c r="D135" s="4"/>
-      <c r="E135" s="4"/>
-      <c r="F135" s="8"/>
-      <c r="G135" s="4"/>
-      <c r="H135" s="4"/>
-      <c r="I135" s="4"/>
+      <c r="A135" s="4">
+        <v>143</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C135" s="8" t="s">
+        <v>1576</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>1542</v>
+      </c>
+      <c r="E135" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>1609</v>
+      </c>
+      <c r="G135" s="4">
+        <v>0</v>
+      </c>
+      <c r="H135" s="4">
+        <v>1</v>
+      </c>
+      <c r="I135" s="4">
+        <v>1</v>
+      </c>
       <c r="J135" s="5"/>
       <c r="K135" s="5"/>
       <c r="L135" s="4"/>
@@ -18396,35 +19439,35 @@
     <row r="2" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str" cm="1">
         <f t="array" aca="1" ref="A2" ca="1">INDEX($A$4:$A$54,RANDBETWEEN(1,COUNTA($A$4:$A$54)),1)</f>
-        <v>NM</v>
+        <v>NH</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)</f>
-        <v>5617178672</v>
+        <v>4646937426</v>
       </c>
       <c r="E2" t="str">
         <f ca="1">RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)&amp;RANDBETWEEN(1,9)</f>
-        <v>84959</v>
+        <v>74111</v>
       </c>
       <c r="G2" t="str" cm="1">
         <f t="array" aca="1" ref="G2" ca="1">(INDEX($H$4:$H$6,RANDBETWEEN(1,COUNTA($H$4:$H$6)),1))&amp;" "&amp;(INDEX($G$4:$G$38,RANDBETWEEN(1,COUNTA($G$4:$G$38)),1))</f>
-        <v>471547 Blake St</v>
+        <v>1567 Lincoln Ave</v>
       </c>
       <c r="J2" t="str" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">INDEX($J$4:$J$6,RANDBETWEEN(1,COUNTA($J$4:$J$6)),1)</f>
-        <v>Diagnose</v>
+        <v>Advisor</v>
       </c>
       <c r="M2" t="str" cm="1">
         <f t="array" aca="1" ref="M2" ca="1">INDEX($M$4:$M$60,RANDBETWEEN(1,COUNTA($M$4:$M$60)),1)</f>
-        <v>Port Huron</v>
+        <v>Manistee</v>
       </c>
       <c r="O2" t="str">
         <f ca="1">IF($R$3=16,$U$37,IF($R$3=17, $U$38,IF($R$3=18,$U$39,IF($R$3=19,$U$40,IF($R$3=20,$U$41,IF($R$3=21,$U$42,IF($R$3=22,$U$43,IF($R$3=23,$U$44,IF($R$3=24,$U$45,IF($R$3=25,$U$46,""))))))))))</f>
-        <v>Phmc5yQU^vS@XK&amp;x^mQpv30</v>
+        <v>CnQEt*povXQ3pBYf@Mr</v>
       </c>
       <c r="P2" s="3">
         <f ca="1">RANDBETWEEN(DATE(1910,1,1),DATE(2021,2,5))</f>
-        <v>17833</v>
+        <v>16625</v>
       </c>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
@@ -18443,23 +19486,23 @@
       <c r="A3" s="12"/>
       <c r="R3" s="5">
         <f ca="1">RANDBETWEEN(16,25)</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="S3" s="4">
         <v>0</v>
       </c>
-      <c r="T3" s="4" t="str" cm="1">
+      <c r="T3" s="4" cm="1">
         <f t="array" aca="1" ref="T3" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>i</v>
+        <v>8</v>
       </c>
       <c r="U3" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T18)</f>
-        <v>iXsriryF43lVRb63</v>
+        <v>8PYFmz3c6VqB0WYM</v>
       </c>
       <c r="V3" s="4"/>
       <c r="W3" s="4" t="str">
         <f ca="1">IF(R3=16,U3,IF(R3=17, U4,IF(R3=18,U5,IF(R3=19,U6,IF(R3=20,U7,IF(R3=21,U8,IF(R3=22,U9,IF(R3=23,U10,IF(R3=24,U11,IF(R3=25,U12,""))))))))))</f>
-        <v>iXsriryF43lVRb63y2a1vhqO</v>
+        <v>8PYFmz3c6VqB0WYMONVr</v>
       </c>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
@@ -18475,7 +19518,7 @@
       </c>
       <c r="H4" t="str">
         <f ca="1">RANDBETWEEN(1,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>7462</v>
+        <v>1567</v>
       </c>
       <c r="J4" t="s">
         <v>275</v>
@@ -18489,11 +19532,11 @@
       </c>
       <c r="T4" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T4" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>X</v>
+        <v>P</v>
       </c>
       <c r="U4" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T19)</f>
-        <v>iXsriryF43lVRb63y</v>
+        <v>8PYFmz3c6VqB0WYMO</v>
       </c>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
@@ -18511,7 +19554,7 @@
       </c>
       <c r="H5" t="str">
         <f ca="1">RANDBETWEEN(1,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>66354</v>
+        <v>12493</v>
       </c>
       <c r="J5" t="s">
         <v>300</v>
@@ -18525,11 +19568,11 @@
       </c>
       <c r="T5" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T5" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>s</v>
+        <v>Y</v>
       </c>
       <c r="U5" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T20)</f>
-        <v>iXsriryF43lVRb63y2</v>
+        <v>8PYFmz3c6VqB0WYMON</v>
       </c>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
@@ -18547,7 +19590,7 @@
       </c>
       <c r="H6" t="str">
         <f ca="1">RANDBETWEEN(1,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>471547</v>
+        <v>719632</v>
       </c>
       <c r="J6" t="s">
         <v>285</v>
@@ -18561,11 +19604,11 @@
       </c>
       <c r="T6" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T6" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>r</v>
+        <v>F</v>
       </c>
       <c r="U6" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T21)</f>
-        <v>iXsriryF43lVRb63y2a</v>
+        <v>8PYFmz3c6VqB0WYMONV</v>
       </c>
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
@@ -18590,11 +19633,11 @@
       </c>
       <c r="T7" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T7" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>i</v>
+        <v>m</v>
       </c>
       <c r="U7" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T22)</f>
-        <v>iXsriryF43lVRb63y2a1</v>
+        <v>8PYFmz3c6VqB0WYMONVr</v>
       </c>
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
@@ -18619,11 +19662,11 @@
       </c>
       <c r="T8" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T8" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>r</v>
+        <v>z</v>
       </c>
       <c r="U8" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T23)</f>
-        <v>iXsriryF43lVRb63y2a1v</v>
+        <v>8PYFmz3c6VqB0WYMONVrI</v>
       </c>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
@@ -18646,13 +19689,13 @@
       <c r="S9" s="4">
         <v>6</v>
       </c>
-      <c r="T9" s="4" t="str" cm="1">
+      <c r="T9" s="4" cm="1">
         <f t="array" aca="1" ref="T9" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>y</v>
+        <v>3</v>
       </c>
       <c r="U9" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T24)</f>
-        <v>iXsriryF43lVRb63y2a1vh</v>
+        <v>8PYFmz3c6VqB0WYMONVrIh</v>
       </c>
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
@@ -18677,11 +19720,11 @@
       </c>
       <c r="T10" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T10" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>F</v>
+        <v>c</v>
       </c>
       <c r="U10" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T25)</f>
-        <v>iXsriryF43lVRb63y2a1vhq</v>
+        <v>8PYFmz3c6VqB0WYMONVrIhO</v>
       </c>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
@@ -18706,11 +19749,11 @@
       </c>
       <c r="T11" s="4" cm="1">
         <f t="array" aca="1" ref="T11" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="U11" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T26)</f>
-        <v>iXsriryF43lVRb63y2a1vhqO</v>
+        <v>8PYFmz3c6VqB0WYMONVrIhOI</v>
       </c>
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
@@ -18733,13 +19776,13 @@
       <c r="S12" s="4">
         <v>9</v>
       </c>
-      <c r="T12" s="4" cm="1">
+      <c r="T12" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T12" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>3</v>
+        <v>V</v>
       </c>
       <c r="U12" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$3:T27)</f>
-        <v>iXsriryF43lVRb63y2a1vhqOF</v>
+        <v>8PYFmz3c6VqB0WYMONVrIhOIV</v>
       </c>
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
@@ -18764,7 +19807,7 @@
       </c>
       <c r="T13" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T13" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>l</v>
+        <v>q</v>
       </c>
       <c r="U13" s="6"/>
       <c r="V13" s="4"/>
@@ -18790,7 +19833,7 @@
       </c>
       <c r="T14" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T14" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>V</v>
+        <v>B</v>
       </c>
       <c r="U14" s="6"/>
       <c r="V14" s="4"/>
@@ -18814,9 +19857,9 @@
       <c r="S15" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="T15" s="4" t="str" cm="1">
+      <c r="T15" s="4" cm="1">
         <f t="array" aca="1" ref="T15" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>R</v>
+        <v>0</v>
       </c>
       <c r="U15" s="6"/>
       <c r="V15" s="4"/>
@@ -18846,7 +19889,7 @@
       </c>
       <c r="T16" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T16" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>b</v>
+        <v>W</v>
       </c>
       <c r="U16" s="6"/>
       <c r="V16" s="4"/>
@@ -18873,9 +19916,9 @@
       <c r="S17" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="T17" s="4" cm="1">
+      <c r="T17" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T17" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>6</v>
+        <v>Y</v>
       </c>
       <c r="U17" s="6"/>
       <c r="V17" s="4"/>
@@ -18899,9 +19942,9 @@
       <c r="S18" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="T18" s="4" cm="1">
+      <c r="T18" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T18" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>3</v>
+        <v>M</v>
       </c>
       <c r="U18" s="6"/>
       <c r="V18" s="4"/>
@@ -18927,7 +19970,7 @@
       </c>
       <c r="T19" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T19" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>y</v>
+        <v>O</v>
       </c>
       <c r="U19" s="6"/>
       <c r="V19" s="4"/>
@@ -18951,9 +19994,9 @@
       <c r="S20" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="T20" s="4" cm="1">
+      <c r="T20" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T20" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>2</v>
+        <v>N</v>
       </c>
       <c r="U20" s="6"/>
       <c r="V20" s="4"/>
@@ -18979,7 +20022,7 @@
       </c>
       <c r="T21" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T21" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>a</v>
+        <v>V</v>
       </c>
       <c r="U21" s="6"/>
       <c r="V21" s="4"/>
@@ -19003,9 +20046,9 @@
       <c r="S22" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="T22" s="4" cm="1">
+      <c r="T22" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T22" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>1</v>
+        <v>r</v>
       </c>
       <c r="U22" s="6"/>
       <c r="V22" s="4"/>
@@ -19031,7 +20074,7 @@
       </c>
       <c r="T23" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T23" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>v</v>
+        <v>I</v>
       </c>
       <c r="U23" s="6"/>
       <c r="V23" s="4"/>
@@ -19083,7 +20126,7 @@
       </c>
       <c r="T25" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T25" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>q</v>
+        <v>O</v>
       </c>
       <c r="U25" s="6"/>
       <c r="V25" s="4"/>
@@ -19109,7 +20152,7 @@
       </c>
       <c r="T26" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T26" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>O</v>
+        <v>I</v>
       </c>
       <c r="U26" s="6"/>
       <c r="V26" s="4"/>
@@ -19135,7 +20178,7 @@
       </c>
       <c r="T27" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T27" ca="1">INDEX($S$3:$S$64,RANDBETWEEN(1,COUNTA($S$3:$S$64)),1)</f>
-        <v>F</v>
+        <v>V</v>
       </c>
       <c r="U27" s="6"/>
       <c r="V27" s="4"/>
@@ -19207,7 +20250,7 @@
       </c>
       <c r="T30" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T30" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>P</v>
+        <v>C</v>
       </c>
       <c r="U30" s="6"/>
       <c r="V30" s="4"/>
@@ -19233,7 +20276,7 @@
       </c>
       <c r="T31" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T31" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>h</v>
+        <v>n</v>
       </c>
       <c r="U31" s="6"/>
       <c r="V31" s="4"/>
@@ -19259,7 +20302,7 @@
       </c>
       <c r="T32" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T32" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>m</v>
+        <v>Q</v>
       </c>
       <c r="U32" s="6"/>
       <c r="V32" s="4"/>
@@ -19285,7 +20328,7 @@
       </c>
       <c r="T33" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T33" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>c</v>
+        <v>E</v>
       </c>
       <c r="U33" s="6"/>
       <c r="V33" s="4"/>
@@ -19309,9 +20352,9 @@
       <c r="S34" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="T34" s="4" cm="1">
+      <c r="T34" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T34" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>5</v>
+        <v>t</v>
       </c>
       <c r="U34" s="6"/>
       <c r="V34" s="4"/>
@@ -19337,7 +20380,7 @@
       </c>
       <c r="T35" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T35" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>y</v>
+        <v>*</v>
       </c>
       <c r="U35" s="6"/>
       <c r="V35" s="4"/>
@@ -19363,7 +20406,7 @@
       </c>
       <c r="T36" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T36" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>Q</v>
+        <v>p</v>
       </c>
       <c r="U36" s="6"/>
       <c r="V36" s="4"/>
@@ -19389,11 +20432,11 @@
       </c>
       <c r="T37" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T37" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>U</v>
+        <v>o</v>
       </c>
       <c r="U37" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T44)</f>
-        <v>Phmc5yQU^vS@XK&amp;</v>
+        <v>CnQEt*povXQ3pBY</v>
       </c>
       <c r="V37" s="4"/>
       <c r="W37" s="4"/>
@@ -19418,11 +20461,11 @@
       </c>
       <c r="T38" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T38" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>^</v>
+        <v>v</v>
       </c>
       <c r="U38" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T45)</f>
-        <v>Phmc5yQU^vS@XK&amp;x</v>
+        <v>CnQEt*povXQ3pBYf</v>
       </c>
       <c r="V38" s="4"/>
       <c r="W38" s="4"/>
@@ -19444,11 +20487,11 @@
       </c>
       <c r="T39" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T39" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>v</v>
+        <v>X</v>
       </c>
       <c r="U39" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T46)</f>
-        <v>Phmc5yQU^vS@XK&amp;x^</v>
+        <v>CnQEt*povXQ3pBYf@</v>
       </c>
       <c r="V39" s="4"/>
       <c r="W39" s="4"/>
@@ -19470,11 +20513,11 @@
       </c>
       <c r="T40" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T40" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>S</v>
+        <v>Q</v>
       </c>
       <c r="U40" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T47)</f>
-        <v>Phmc5yQU^vS@XK&amp;x^m</v>
+        <v>CnQEt*povXQ3pBYf@M</v>
       </c>
       <c r="V40" s="4"/>
       <c r="W40" s="4"/>
@@ -19494,13 +20537,13 @@
       <c r="S41" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="T41" s="4" t="str" cm="1">
+      <c r="T41" s="4" cm="1">
         <f t="array" aca="1" ref="T41" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>@</v>
+        <v>3</v>
       </c>
       <c r="U41" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T48)</f>
-        <v>Phmc5yQU^vS@XK&amp;x^mQ</v>
+        <v>CnQEt*povXQ3pBYf@Mr</v>
       </c>
       <c r="V41" s="4"/>
       <c r="W41" s="4"/>
@@ -19522,11 +20565,11 @@
       </c>
       <c r="T42" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T42" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>X</v>
+        <v>p</v>
       </c>
       <c r="U42" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T49)</f>
-        <v>Phmc5yQU^vS@XK&amp;x^mQp</v>
+        <v>CnQEt*povXQ3pBYf@MrV</v>
       </c>
       <c r="V42" s="4"/>
       <c r="W42" s="4"/>
@@ -19548,11 +20591,11 @@
       </c>
       <c r="T43" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T43" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>K</v>
+        <v>B</v>
       </c>
       <c r="U43" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T50)</f>
-        <v>Phmc5yQU^vS@XK&amp;x^mQpv</v>
+        <v>CnQEt*povXQ3pBYf@MrV$</v>
       </c>
       <c r="V43" s="4"/>
       <c r="W43" s="4"/>
@@ -19574,11 +20617,11 @@
       </c>
       <c r="T44" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T44" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>&amp;</v>
+        <v>Y</v>
       </c>
       <c r="U44" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T51)</f>
-        <v>Phmc5yQU^vS@XK&amp;x^mQpv3</v>
+        <v>CnQEt*povXQ3pBYf@MrV$@</v>
       </c>
       <c r="V44" s="4"/>
       <c r="W44" s="4"/>
@@ -19600,11 +20643,11 @@
       </c>
       <c r="T45" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T45" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>x</v>
+        <v>f</v>
       </c>
       <c r="U45" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T52)</f>
-        <v>Phmc5yQU^vS@XK&amp;x^mQpv30</v>
+        <v>CnQEt*povXQ3pBYf@MrV$@c</v>
       </c>
       <c r="V45" s="4"/>
       <c r="W45" s="4"/>
@@ -19626,11 +20669,11 @@
       </c>
       <c r="T46" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T46" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>^</v>
+        <v>@</v>
       </c>
       <c r="U46" s="6" t="str">
         <f ca="1">_xlfn.CONCAT($T$30:T53)</f>
-        <v>Phmc5yQU^vS@XK&amp;x^mQpv306</v>
+        <v>CnQEt*povXQ3pBYf@MrV$@cd</v>
       </c>
       <c r="V46" s="4"/>
       <c r="W46" s="4"/>
@@ -19652,7 +20695,7 @@
       </c>
       <c r="T47" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T47" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>m</v>
+        <v>M</v>
       </c>
       <c r="U47" s="6"/>
       <c r="V47" s="4"/>
@@ -19675,7 +20718,7 @@
       </c>
       <c r="T48" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T48" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>Q</v>
+        <v>r</v>
       </c>
       <c r="U48" s="6"/>
       <c r="V48" s="4"/>
@@ -19698,7 +20741,7 @@
       </c>
       <c r="T49" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T49" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>p</v>
+        <v>V</v>
       </c>
       <c r="U49" s="6"/>
       <c r="V49" s="4"/>
@@ -19721,7 +20764,7 @@
       </c>
       <c r="T50" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T50" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>v</v>
+        <v>$</v>
       </c>
       <c r="U50" s="6"/>
       <c r="V50" s="4"/>
@@ -19742,9 +20785,9 @@
       <c r="S51" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="T51" s="4" cm="1">
+      <c r="T51" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T51" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>3</v>
+        <v>@</v>
       </c>
       <c r="U51" s="6"/>
       <c r="V51" s="4"/>
@@ -19765,9 +20808,9 @@
       <c r="S52" s="4" t="s">
         <v>612</v>
       </c>
-      <c r="T52" s="4" cm="1">
+      <c r="T52" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T52" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>0</v>
+        <v>c</v>
       </c>
       <c r="U52" s="6"/>
       <c r="V52" s="4"/>
@@ -19788,9 +20831,9 @@
       <c r="S53" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="T53" s="4" cm="1">
+      <c r="T53" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="T53" ca="1">INDEX($S$3:$S$72,RANDBETWEEN(1,COUNTA($S$3:$S$72)),1)</f>
-        <v>6</v>
+        <v>d</v>
       </c>
       <c r="V53" s="4"/>
       <c r="W53" s="4"/>
@@ -20033,8 +21076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B78DEF-5A20-47DD-A1BF-E039EC331573}">
   <dimension ref="A1:AK122"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:R1048576"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="Q103" sqref="Q103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26838,7 +27881,60 @@
       <c r="V102" s="13"/>
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O103" s="2"/>
+      <c r="A103">
+        <v>110</v>
+      </c>
+      <c r="B103" s="2">
+        <v>106245963</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>1509</v>
+      </c>
+      <c r="D103" t="s">
+        <v>251</v>
+      </c>
+      <c r="E103" t="s">
+        <v>252</v>
+      </c>
+      <c r="F103" t="s">
+        <v>139</v>
+      </c>
+      <c r="G103" s="3">
+        <v>6880</v>
+      </c>
+      <c r="H103" t="s">
+        <v>653</v>
+      </c>
+      <c r="I103">
+        <v>194</v>
+      </c>
+      <c r="J103" s="5">
+        <v>72.569999999999993</v>
+      </c>
+      <c r="K103" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="L103" t="s">
+        <v>337</v>
+      </c>
+      <c r="M103" t="s">
+        <v>430</v>
+      </c>
+      <c r="N103" s="2">
+        <v>69232</v>
+      </c>
+      <c r="O103" s="2">
+        <v>5399295221</v>
+      </c>
+      <c r="P103" s="18" t="s">
+        <v>830</v>
+      </c>
+      <c r="Q103">
+        <v>52</v>
+      </c>
+      <c r="R103">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" s="9"/>
@@ -27212,42 +28308,66 @@
     <mergeCell ref="T110:W111"/>
     <mergeCell ref="T112:W113"/>
   </mergeCells>
-  <conditionalFormatting sqref="P1:P105 P123:P1048576">
+  <conditionalFormatting sqref="P1:P102 P123:P1048576 P104:P105">
+    <cfRule type="duplicateValues" dxfId="54" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:C102 B123:C1048576 B104:C105">
+    <cfRule type="duplicateValues" dxfId="53" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C102 C123:C1048576 C104:C105">
+    <cfRule type="duplicateValues" dxfId="52" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B102 B123:B1048576 B104:B105">
+    <cfRule type="duplicateValues" dxfId="51" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P106:P122">
+    <cfRule type="duplicateValues" dxfId="50" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B106:C122">
+    <cfRule type="duplicateValues" dxfId="49" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C106:C122">
+    <cfRule type="duplicateValues" dxfId="48" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B106:B122">
     <cfRule type="duplicateValues" dxfId="47" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C105 B123:C1048576">
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="46" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C105 C123:C1048576">
+  <conditionalFormatting sqref="B1:B102 B104:B1048576">
     <cfRule type="duplicateValues" dxfId="45" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B105 B123:B1048576">
+  <conditionalFormatting sqref="C1:C102 C104:C1048576">
     <cfRule type="duplicateValues" dxfId="44" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P106:P122">
+  <conditionalFormatting sqref="P1:P102 P104:P1048576">
     <cfRule type="duplicateValues" dxfId="43" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B106:C122">
+  <conditionalFormatting sqref="P103">
     <cfRule type="duplicateValues" dxfId="42" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C106:C122">
+  <conditionalFormatting sqref="B103:C103">
     <cfRule type="duplicateValues" dxfId="41" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B106:B122">
+  <conditionalFormatting sqref="C103">
     <cfRule type="duplicateValues" dxfId="40" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
+  <conditionalFormatting sqref="B103">
     <cfRule type="duplicateValues" dxfId="39" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B103">
     <cfRule type="duplicateValues" dxfId="38" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C103">
     <cfRule type="duplicateValues" dxfId="37" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1048576">
+  <conditionalFormatting sqref="P103">
     <cfRule type="duplicateValues" dxfId="36" priority="1"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="P103" r:id="rId1" xr:uid="{C7E52701-A2BC-4D91-86B1-DC28349F9842}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -32566,7 +33686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5AC3597-E535-4CA0-AB6F-F14E144696CA}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
@@ -33704,21 +34824,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CECBC2A9D97CCE4C8584DF116D967F1C" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bccd6ae8185a02004a5a45138277f666">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7be332c0-1dcf-4a8f-9aaa-d80332f69483" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1268db3e156c331756c14e9fb6f811d7" ns2:_="">
     <xsd:import namespace="7be332c0-1dcf-4a8f-9aaa-d80332f69483"/>
@@ -33890,31 +34995,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49942C0E-E08D-4759-9E7E-944B12612524}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="7be332c0-1dcf-4a8f-9aaa-d80332f69483"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F957795-5A4E-4E04-BFAB-7B388D638E5F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D315D914-8530-49D9-AF00-9C03EBB80621}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33932,6 +35028,30 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F957795-5A4E-4E04-BFAB-7B388D638E5F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49942C0E-E08D-4759-9E7E-944B12612524}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7be332c0-1dcf-4a8f-9aaa-d80332f69483"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=userCustomization/customUI.xml><?xml version="1.0" encoding="utf-8"?>
 <mso:customUI xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui">
   <mso:ribbon>

</xml_diff>